<commit_message>
added ftdi chip and supporting components to design.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="164">
   <si>
     <t>Section</t>
   </si>
@@ -301,13 +301,221 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-search/en?v=490&amp;FV=fff40002%2Cfff8000b%2C1c0002%2C34006f%2C380020%2C400005%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>USART&lt;-&gt;USB COM</t>
+  </si>
+  <si>
+    <t>FT232HL-REEL</t>
+  </si>
+  <si>
+    <t>768-1101-1-ND</t>
+  </si>
+  <si>
+    <t>IC HS USB TO UART/FIFO 48LQFP</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/FT232HL-REEL/768-1101-1-ND/2614632</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>API Develan</t>
+  </si>
+  <si>
+    <t>SDS850R-104M</t>
+  </si>
+  <si>
+    <t>100uH</t>
+  </si>
+  <si>
+    <t>FIXED IND 100UH 500MA 600 MOHM</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv314=3313&amp;FV=fff40003%2Cfff80013%2C1c0002%2C1c0003%2C108002f%2C1400008&amp;k=INDUCTOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>GRM1885C2A4R7CA01D</t>
+  </si>
+  <si>
+    <t>490-6392-1-ND</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7PF 100V NP0 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv405=19&amp;FV=fff40002%2Cfff8000b%2Cfffc01ea%2C1c0002%2C3400af%2C380002%2C380004%2C380009%2C380014%2C380016%2C380020%2C400005%2C400006%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF3902V</t>
+  </si>
+  <si>
+    <t>P39.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>RES SMD 39K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=1044&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1202V</t>
+  </si>
+  <si>
+    <t>P12.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>12k</t>
+  </si>
+  <si>
+    <t>RES SMD 12K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=1029&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>93LC56BT-I/OT</t>
+  </si>
+  <si>
+    <t>93LC56BT-I/OTCT-ND</t>
+  </si>
+  <si>
+    <t>IC EEPROM 2KBIT 2MHZ SOT23-6</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=93lc56bt-i%2Fot-&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2001V</t>
+  </si>
+  <si>
+    <t>P2.00KHCT-ND</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=380&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ZX62WD1-B-5PC/H12193CT-ND/3761044</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>Hirose</t>
+  </si>
+  <si>
+    <t>CONN RCPT MICRO USB B SPLASH PRF</t>
+  </si>
+  <si>
+    <t>ZX62WD1-B-5PC</t>
+  </si>
+  <si>
+    <t>H12193CT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3GEY0R00V</t>
+  </si>
+  <si>
+    <t>P0.0GCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0 OHM JUMPER 1/10W</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1291=1036&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C40400%2C1c0002&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>12MHz</t>
+  </si>
+  <si>
+    <t>9C-12.000MAAJ-T</t>
+  </si>
+  <si>
+    <t>887-1053-1-ND</t>
+  </si>
+  <si>
+    <t>CRYSTAL 12MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv16=319&amp;FV=fff4000d%2Cfff8016d%2Cfffc0377%2C1c0002%2C1c0003%2C1140003%2C22c019d%2C3f40008%2C8640004%2Cb5005c0&amp;k=CRYSTAL&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2200V</t>
+  </si>
+  <si>
+    <t>P220HCT-ND</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>RES SMD 220 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1=310&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>LITE-ON</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LTST-C193KRKT-5A/160-1830-1-ND/2356251</t>
+  </si>
+  <si>
+    <t>LED RED RECT CLEAR 0603</t>
+  </si>
+  <si>
+    <t>LTST-C193KRKT-5A</t>
+  </si>
+  <si>
+    <t>MCU/IO
+FTDI</t>
+  </si>
+  <si>
+    <t>TVS</t>
+  </si>
+  <si>
+    <t>Littlefuse</t>
+  </si>
+  <si>
+    <t>PGB1010603MR</t>
+  </si>
+  <si>
+    <t>F2594CT-ND</t>
+  </si>
+  <si>
+    <t>TVS DIODE 24VWM 150VC 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/PGB1010603MR/F2594CT-ND/813072</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +533,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -350,10 +564,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +875,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,12 +888,12 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -869,12 +1090,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -904,12 +1125,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
@@ -974,12 +1195,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
@@ -1009,9 +1230,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1049,7 +1270,7 @@
         <v>43</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>84</v>
@@ -1079,12 +1300,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>50</v>
@@ -1182,6 +1403,461 @@
       </c>
       <c r="K17" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18">
+        <v>4.25</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19">
+        <v>2.48</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20">
+        <v>0.24</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22">
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23">
+        <v>0.27</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24">
+        <v>0.1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>137</v>
+      </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0.1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27">
+        <v>0.44</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I28">
+        <v>0.1</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D29" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>156</v>
+      </c>
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29">
+        <v>0.43</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30">
+        <v>0.67</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K30" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added adc and supporting components
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="720" yWindow="360" windowWidth="22755" windowHeight="10260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="ADC" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="183">
   <si>
     <t>Section</t>
   </si>
@@ -129,22 +129,7 @@
     <t>ADA4610-2ARMZ</t>
   </si>
   <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>FTDI chip</t>
-  </si>
-  <si>
     <t>FTDI</t>
-  </si>
-  <si>
-    <t>FT230XS-R</t>
-  </si>
-  <si>
-    <t>768-1135-1-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=ffec6a38%2Cffec80d2%2Cfff40027%2Cfff80319%2Cfffc0300%2C1c0000%2C1c0002%2C1c0003%2C1c0006%2C1c0011%2C40326f%2C403305%2C403311%2C268003e%2C2680073%2C268036b%2C3f00002%2C4500013%2C450001e%2C450004f%2C4500127%2C45002af%2C45003ef%2C45004f1%2C4500565%2C45005b2%2C450090d%2C4500b99%2C9080092%2C920002f%2C142c00c1&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
     <t>MCU/IO</t>
@@ -509,13 +494,87 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/PGB1010603MR/F2594CT-ND/813072</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t># Channels</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t># Sim Channels</t>
+  </si>
+  <si>
+    <t>AD7656</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>SPS</t>
+  </si>
+  <si>
+    <t>250k</t>
+  </si>
+  <si>
+    <t>Vin Range</t>
+  </si>
+  <si>
+    <t>[-5,5]</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>http://www.analog.com/static/imported-files/data_sheets/AD7656_7657_7658.pdf</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>AD7656YSTZ</t>
+  </si>
+  <si>
+    <t>AD7656YSTZ-ND</t>
+  </si>
+  <si>
+    <t>IC ADC 16BIT 6CH 250KSPS 64LQFP</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/AD7656YSTZ/AD7656YSTZ-ND/1132271</t>
+  </si>
+  <si>
+    <t>MCU/IO
+FTDI
+ADC</t>
+  </si>
+  <si>
+    <t>C1608X5R1E106M080AC</t>
+  </si>
+  <si>
+    <t>445-9015-1-ND</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V 20% X5R 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?v=445&amp;FV=fff40002%2Cfff8000b%2C1c0002%2C340045%2C380014%2C400005%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,12 +592,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -564,13 +617,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -875,11 +925,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1067,108 +1117,120 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8">
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8">
+        <v>0.1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>157</v>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I9">
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10">
+        <v>0.44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
         <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10">
-        <v>0.1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
       </c>
       <c r="D11" t="s">
         <v>59</v>
@@ -1186,27 +1248,27 @@
         <v>62</v>
       </c>
       <c r="I11">
-        <v>0.44</v>
+        <v>0.16</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>157</v>
+      <c r="A12" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>65</v>
@@ -1217,188 +1279,188 @@
       <c r="G12" t="s">
         <v>66</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <v>549</v>
+      </c>
+      <c r="I12">
+        <v>0.1</v>
+      </c>
+      <c r="J12" t="s">
         <v>67</v>
       </c>
-      <c r="I12">
-        <v>0.16</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>68</v>
       </c>
-      <c r="K12" t="s">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13">
+        <v>1.51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
         <v>70</v>
       </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13">
-        <v>549</v>
-      </c>
-      <c r="I13">
-        <v>0.1</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
         <v>72</v>
       </c>
-      <c r="K13" t="s">
+      <c r="H15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14">
-        <v>1.51</v>
-      </c>
-      <c r="J14" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I15">
+        <v>0.24</v>
+      </c>
+      <c r="J15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="K15" t="s">
         <v>75</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15">
-        <v>0.1</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I16">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="K16" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I17">
-        <v>0.1</v>
-      </c>
-      <c r="J17" t="s">
+        <v>4.25</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>93</v>
       </c>
       <c r="K17" t="s">
@@ -1406,20 +1468,20 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
+      <c r="A18" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -1428,33 +1490,33 @@
         <v>97</v>
       </c>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="I18">
-        <v>4.25</v>
+        <v>2.48</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>39</v>
+      <c r="A19" t="s">
+        <v>37</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
         <v>101</v>
-      </c>
-      <c r="E19" t="s">
-        <v>102</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1466,7 +1528,7 @@
         <v>103</v>
       </c>
       <c r="I19">
-        <v>2.48</v>
+        <v>0.24</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>104</v>
@@ -1477,16 +1539,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>106</v>
@@ -1501,7 +1563,7 @@
         <v>108</v>
       </c>
       <c r="I20">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>109</v>
@@ -1512,7 +1574,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1547,66 +1609,66 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="I22">
-        <v>0.1</v>
+        <v>0.27</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
         <v>122</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
         <v>123</v>
       </c>
-      <c r="F23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>124</v>
       </c>
-      <c r="H23" t="s">
-        <v>88</v>
-      </c>
       <c r="I23">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>125</v>
@@ -1617,86 +1679,86 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H24" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="I24">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>130</v>
       </c>
       <c r="K24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
         <v>133</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
         <v>134</v>
       </c>
-      <c r="E25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" t="s">
-        <v>137</v>
-      </c>
-      <c r="H25" t="s">
-        <v>88</v>
+      <c r="H25">
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>135</v>
       </c>
       <c r="K25" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
         <v>138</v>
@@ -1707,11 +1769,11 @@
       <c r="G26" t="s">
         <v>139</v>
       </c>
-      <c r="H26">
-        <v>0</v>
+      <c r="H26" t="s">
+        <v>137</v>
       </c>
       <c r="I26">
-        <v>0.1</v>
+        <v>0.44</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>140</v>
@@ -1722,31 +1784,31 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
         <v>143</v>
       </c>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>144</v>
       </c>
-      <c r="H27" t="s">
-        <v>142</v>
-      </c>
       <c r="I27">
-        <v>0.44</v>
+        <v>0.1</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>145</v>
@@ -1757,54 +1819,54 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H28" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="I28">
-        <v>0.1</v>
+        <v>0.43</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>150</v>
       </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -1813,51 +1875,86 @@
         <v>156</v>
       </c>
       <c r="H29" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I29">
-        <v>0.43</v>
+        <v>0.67</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K29" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>172</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>160</v>
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>173</v>
       </c>
       <c r="F30" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>161</v>
+      <c r="G30" t="s">
+        <v>174</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I30">
-        <v>0.67</v>
+        <v>25.16</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="K30" t="s">
-        <v>163</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" t="s">
+        <v>180</v>
+      </c>
+      <c r="I31">
+        <v>0.89</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K31" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1866,21 +1963,92 @@
     <hyperlink ref="K4" r:id="rId2"/>
     <hyperlink ref="K5" r:id="rId3"/>
     <hyperlink ref="K6" r:id="rId4"/>
-    <hyperlink ref="K8" r:id="rId5" display="http://www.digikey.com/product-search/en?pv7=2&amp;FV=ffec6a38%2Cffec80d2%2Cfff40027%2Cfff80319%2Cfffc0300%2C1c0000%2C1c0002%2C1c0003%2C1c0006%2C1c0011%2C40326f%2C403305%2C403311%2C268003e%2C2680073%2C268036b%2C3f00002%2C4500013%2C450001e%2C450004f%2C4500127%2C45002af%2C45003ef%2C45004f1%2C4500565%2C45005b2%2C450090d%2C4500b99%2C9080092%2C920002f%2C142c00c1&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="76.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added temperature sensor and supporting components
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="190">
   <si>
     <t>Section</t>
   </si>
@@ -550,24 +550,47 @@
     <t>http://www.digikey.com/product-detail/en/AD7656YSTZ/AD7656YSTZ-ND/1132271</t>
   </si>
   <si>
+    <t>C1608X5R1E106M080AC</t>
+  </si>
+  <si>
+    <t>445-9015-1-ND</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V 20% X5R 0603</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?v=445&amp;FV=fff40002%2Cfff8000b%2C1c0002%2C340045%2C380014%2C400005%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>ADC
+TEMP</t>
+  </si>
+  <si>
     <t>MCU/IO
 FTDI
-ADC</t>
-  </si>
-  <si>
-    <t>C1608X5R1E106M080AC</t>
-  </si>
-  <si>
-    <t>445-9015-1-ND</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 25V 20% X5R 0603</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?v=445&amp;FV=fff40002%2Cfff8000b%2C1c0002%2C340045%2C380014%2C400005%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+ADC
+TEMP</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>MCP9700AT-E/TT</t>
+  </si>
+  <si>
+    <t>MCP9700AT-E/TTCT-ND</t>
+  </si>
+  <si>
+    <t>IC SENSOR THERMAL 2.3V SOT-23-3</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv1291=88&amp;FV=fff4001e%2Cfff80137%2C1c0002%2C1c0003%2C378008e&amp;k=mcp9700&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
 </sst>
 </file>
@@ -925,11 +948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,12 +1140,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -1152,12 +1175,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B9">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1922,12 +1945,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>172</v>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="B31">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
@@ -1936,25 +1959,60 @@
         <v>46</v>
       </c>
       <c r="E31" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
         <v>178</v>
       </c>
-      <c r="F31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>179</v>
-      </c>
-      <c r="H31" t="s">
-        <v>180</v>
       </c>
       <c r="I31">
         <v>0.89</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K31" t="s">
         <v>181</v>
       </c>
-      <c r="K31" t="s">
-        <v>182</v>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>187</v>
+      </c>
+      <c r="H32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32">
+        <v>0.37</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K32" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed op amp broken link.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -1268,9 +1268,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1354,10 +1352,10 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1389,10 +1387,10 @@
         <v>2</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1424,10 +1422,10 @@
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>3</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1459,10 +1457,10 @@
         <v>2</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1494,10 +1492,10 @@
         <v>2</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1529,10 +1527,10 @@
         <v>2</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1564,10 +1562,10 @@
         <v>2</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1599,10 +1597,10 @@
         <v>2</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1634,10 +1632,10 @@
         <v>2</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1669,10 +1667,10 @@
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1704,10 +1702,10 @@
         <v>2</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1739,10 +1737,10 @@
         <v>2</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1774,10 +1772,10 @@
         <v>2</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1809,10 +1807,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1949,10 +1947,10 @@
         <v>2</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1984,10 +1982,10 @@
         <v>2</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2019,10 +2017,10 @@
         <v>2</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2054,10 +2052,10 @@
         <v>2</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2089,7 +2087,7 @@
         <v>3</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>3</v>
@@ -2159,10 +2157,10 @@
         <v>2</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>220</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2194,10 +2192,10 @@
         <v>2</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>212</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2229,10 +2227,10 @@
         <v>2</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2264,10 +2262,10 @@
         <v>2</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2299,10 +2297,10 @@
         <v>2</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2334,10 +2332,10 @@
         <v>2</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2369,10 +2367,10 @@
         <v>2</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>215</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2439,10 +2437,10 @@
         <v>2</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>271</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2474,10 +2472,10 @@
         <v>2</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2509,10 +2507,10 @@
         <v>2</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>269</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2544,10 +2542,10 @@
         <v>2</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2579,10 +2577,10 @@
         <v>2</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2614,10 +2612,10 @@
         <v>2</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2649,10 +2647,10 @@
         <v>2</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2684,10 +2682,10 @@
         <v>2</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2719,10 +2717,10 @@
         <v>2</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2754,10 +2752,10 @@
         <v>2</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2789,10 +2787,10 @@
         <v>2</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2824,14 +2822,14 @@
         <v>2</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I44">
+  <sortState ref="A2:K44">
     <sortCondition ref="F2:F44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed broken or wrong links.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -21,24 +21,576 @@
     <t>Number</t>
   </si>
   <si>
+    <t>Mfg Part Number</t>
+  </si>
+  <si>
+    <t>FT232HL-REEL</t>
+  </si>
+  <si>
+    <t>SDS850R-104M</t>
+  </si>
+  <si>
+    <t>GRM1885C2A4R7CA01D</t>
+  </si>
+  <si>
+    <t>C1608X7R1E104K080AA</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF3902V</t>
+  </si>
+  <si>
+    <t>KS11R22CQD</t>
+  </si>
+  <si>
+    <t>C1608X7R1E105K080AB</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1202V</t>
+  </si>
+  <si>
+    <t>93LC56BT-I/OT</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1002V</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2001V</t>
+  </si>
+  <si>
+    <t>ZX80-B-5P</t>
+  </si>
+  <si>
+    <t>ERJ-3GEY0R00V</t>
+  </si>
+  <si>
+    <t>PGB1010603MR</t>
+  </si>
+  <si>
+    <t>9C-12.000MAAJ-T</t>
+  </si>
+  <si>
+    <t>GRM1885C1H180FA01D</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF5490V</t>
+  </si>
+  <si>
+    <t>LTST-C193KRKT-5A</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2200V</t>
+  </si>
+  <si>
+    <t>9C-16.000MAAJ-T</t>
+  </si>
+  <si>
+    <t>GRM1885C1H2R2CA01D</t>
+  </si>
+  <si>
+    <t>STM32F401VCT6</t>
+  </si>
+  <si>
+    <t>TLV1702AIDGKR</t>
+  </si>
+  <si>
+    <t>&lt;null&gt;</t>
+  </si>
+  <si>
+    <t>AD8277ARZ-RL</t>
+  </si>
+  <si>
+    <t>LOC111PTR</t>
+  </si>
+  <si>
+    <t>PLTT0805Z4990QGT5</t>
+  </si>
+  <si>
+    <t>OPA602BP</t>
+  </si>
+  <si>
+    <t>PLTT0805Z5002QGT5</t>
+  </si>
+  <si>
+    <t>PLTT0805Z2002QGT5</t>
+  </si>
+  <si>
+    <t>AD7656BSTZ-REEL</t>
+  </si>
+  <si>
+    <t>C1608X5R1E106M080AC</t>
+  </si>
+  <si>
+    <t>MCP9700AT-E/TT</t>
+  </si>
+  <si>
+    <t>HE3621A0510</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1000V</t>
+  </si>
+  <si>
+    <t>ERA-8AEB124V</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2202V</t>
+  </si>
+  <si>
+    <t>310-87-102-41-001101</t>
+  </si>
+  <si>
+    <t>AD817ARZ-REEL7</t>
+  </si>
+  <si>
+    <t>AD5640BRJZ-1500RL7</t>
+  </si>
+  <si>
+    <t>TLV341AIDBVR</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>FTDI</t>
+  </si>
+  <si>
+    <t>API Develan</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>Hirose</t>
+  </si>
+  <si>
+    <t>Littlefuse</t>
+  </si>
+  <si>
+    <t>TXC</t>
+  </si>
+  <si>
+    <t>LITE-ON</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>IXYS</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>Preci-Dip</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>FT232H</t>
+  </si>
+  <si>
+    <t>100uH</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>39K</t>
+  </si>
+  <si>
+    <t>SW_PUSHBUTTON_SPST</t>
+  </si>
+  <si>
+    <t>12k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>USB-MICRO-B</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>DIODE_TS_BI_DIR</t>
+  </si>
+  <si>
+    <t>12MHz</t>
+  </si>
+  <si>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>549R</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>STM32F401</t>
+  </si>
+  <si>
+    <t>JTAG</t>
+  </si>
+  <si>
+    <t>TLV1702</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>AD8277</t>
+  </si>
+  <si>
+    <t>BNC</t>
+  </si>
+  <si>
+    <t>LOC111</t>
+  </si>
+  <si>
+    <t>499R-check</t>
+  </si>
+  <si>
+    <t>OPA602</t>
+  </si>
+  <si>
+    <t>50k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>AD7656</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>MCP9700AT</t>
+  </si>
+  <si>
+    <t>HE3621_NO_SPST</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>120K</t>
+  </si>
+  <si>
+    <t>22k</t>
+  </si>
+  <si>
+    <t>CON2</t>
+  </si>
+  <si>
+    <t>AD817</t>
+  </si>
+  <si>
+    <t>AD5640</t>
+  </si>
+  <si>
+    <t>TLV341</t>
+  </si>
+  <si>
+    <t>Part Type</t>
+  </si>
+  <si>
+    <t>USB COM</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>Push Button</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>TVS</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>Op Amp</t>
+  </si>
+  <si>
+    <t>Diff Amp</t>
+  </si>
+  <si>
+    <t>Optocoupler</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Temperature Sensor</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>Part Reference</t>
+  </si>
+  <si>
+    <t>U20</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>U21</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>U19</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>IC HS USB TO UART/FIFO 48LQFP</t>
+  </si>
+  <si>
+    <t>FIXED IND 100UH 500MA 600 MOHM</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7PF 100V NP0 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 39K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>SWITCH PUSH SPST-NO 0.025A 50V</t>
+  </si>
+  <si>
+    <t>RES SMD 12K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>IC EEPROM 2KBIT 2MHZ SOT23-6</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CONN RCPT MICRO USB B PCB VERT</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0 OHM JUMPER 1/10W</t>
+  </si>
+  <si>
+    <t>TVS DIODE 24VWM 150VC 0603</t>
+  </si>
+  <si>
+    <t>CRYSTAL 12MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>CAP CER 18PF 50V 1% NP0 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 549 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>LED RED RECT CLEAR 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 220 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2PF 50V NP0 0603</t>
+  </si>
+  <si>
+    <t>IC MCU ARM M4 32BIT RISC 100LQFP</t>
+  </si>
+  <si>
+    <t>CONN RCPT 20POS VERT DL 2.54MM</t>
+  </si>
+  <si>
+    <t>IC COMPARATOR DUAL 8VSSOP</t>
+  </si>
+  <si>
+    <t>IC OPAMP DIFF 550KHZ RRO 14SOIC</t>
+  </si>
+  <si>
+    <t>CONN BNC JACK STR 50 OHM PCB</t>
+  </si>
+  <si>
+    <t>OPTOISO 3.75KV PHVOLT 8-FLATPACK</t>
+  </si>
+  <si>
+    <t>RES SMD 499 OHM 0.02% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 6.5MHZ 8DIP</t>
+  </si>
+  <si>
+    <t>RES SMD 50K OHM 0.02% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 20K OHM 0.02% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>IC ADC 16BIT 6CH 250KSPS 64-LQFP</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V 20% X5R 0603</t>
+  </si>
+  <si>
+    <t>IC SENSOR THERMAL 2.3V SOT-23-3</t>
+  </si>
+  <si>
+    <t>RELAY REED SPST 500MA 5V</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 120K OHM 0.1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RES SMD 22K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>SOCKET 4.2 MM SOLDER TAIL SINGLE</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 50MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>IC DAC 14BIT SPI/SRL SOT23-8</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 2.3MHZ RRO SOT23-6</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
     <t>Supplier</t>
   </si>
   <si>
     <t>Digikey</t>
   </si>
   <si>
-    <t>&lt;null&gt;</t>
-  </si>
-  <si>
     <t>Supplier Part Number</t>
   </si>
   <si>
     <t>768-1101-1-ND</t>
   </si>
   <si>
-    <t>SDS850R-104M</t>
-  </si>
-  <si>
     <t>490-6392-1-ND</t>
   </si>
   <si>
@@ -159,558 +711,27 @@
     <t>296-17680-1-ND</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>FTDI</t>
-  </si>
-  <si>
-    <t>API Develan</t>
-  </si>
-  <si>
-    <t>Murata</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>C&amp;K</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>Hirose</t>
-  </si>
-  <si>
-    <t>Littlefuse</t>
-  </si>
-  <si>
-    <t>TXC</t>
-  </si>
-  <si>
-    <t>LITE-ON</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>Analog Devices</t>
-  </si>
-  <si>
-    <t>IXYS</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>Preci-Dip</t>
-  </si>
-  <si>
-    <t>Mfg Part Number</t>
-  </si>
-  <si>
-    <t>FT232HL-REEL</t>
-  </si>
-  <si>
-    <t>GRM1885C2A4R7CA01D</t>
-  </si>
-  <si>
-    <t>C1608X7R1E104K080AA</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF3902V</t>
-  </si>
-  <si>
-    <t>KS11R22CQD</t>
-  </si>
-  <si>
-    <t>C1608X7R1E105K080AB</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1202V</t>
-  </si>
-  <si>
-    <t>93LC56BT-I/OT</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2001V</t>
-  </si>
-  <si>
-    <t>ZX80-B-5P</t>
-  </si>
-  <si>
-    <t>ERJ-3GEY0R00V</t>
-  </si>
-  <si>
-    <t>PGB1010603MR</t>
-  </si>
-  <si>
-    <t>9C-12.000MAAJ-T</t>
-  </si>
-  <si>
-    <t>GRM1885C1H180FA01D</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF5490V</t>
-  </si>
-  <si>
-    <t>LTST-C193KRKT-5A</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2200V</t>
-  </si>
-  <si>
-    <t>9C-16.000MAAJ-T</t>
-  </si>
-  <si>
-    <t>GRM1885C1H2R2CA01D</t>
-  </si>
-  <si>
-    <t>STM32F401VCT6</t>
-  </si>
-  <si>
-    <t>TLV1702AIDGKR</t>
-  </si>
-  <si>
-    <t>AD8277ARZ-RL</t>
-  </si>
-  <si>
-    <t>LOC111PTR</t>
-  </si>
-  <si>
-    <t>PLTT0805Z4990QGT5</t>
-  </si>
-  <si>
-    <t>OPA602BP</t>
-  </si>
-  <si>
-    <t>PLTT0805Z5002QGT5</t>
-  </si>
-  <si>
-    <t>PLTT0805Z2002QGT5</t>
-  </si>
-  <si>
-    <t>AD7656BSTZ-REEL</t>
-  </si>
-  <si>
-    <t>C1608X5R1E106M080AC</t>
-  </si>
-  <si>
-    <t>MCP9700AT-E/TT</t>
-  </si>
-  <si>
-    <t>HE3621A0510</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1000V</t>
-  </si>
-  <si>
-    <t>ERA-8AEB124V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2202V</t>
-  </si>
-  <si>
-    <t>310-87-102-41-001101</t>
-  </si>
-  <si>
-    <t>AD817ARZ-REEL7</t>
-  </si>
-  <si>
-    <t>AD5640BRJZ-1500RL7</t>
-  </si>
-  <si>
-    <t>TLV341AIDBVR</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>FT232H</t>
-  </si>
-  <si>
-    <t>100uH</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>39K</t>
-  </si>
-  <si>
-    <t>SW_PUSHBUTTON_SPST</t>
-  </si>
-  <si>
-    <t>12k</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>2K</t>
-  </si>
-  <si>
-    <t>USB-MICRO-B</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>DIODE_TS_BI_DIR</t>
-  </si>
-  <si>
-    <t>12MHz</t>
-  </si>
-  <si>
-    <t>18pF</t>
-  </si>
-  <si>
-    <t>549R</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>16MHz</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>STM32F401</t>
-  </si>
-  <si>
-    <t>JTAG</t>
-  </si>
-  <si>
-    <t>TLV1702</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>AD8277</t>
-  </si>
-  <si>
-    <t>BNC</t>
-  </si>
-  <si>
-    <t>LOC111</t>
-  </si>
-  <si>
-    <t>499R-check</t>
-  </si>
-  <si>
-    <t>OPA602</t>
-  </si>
-  <si>
-    <t>50k</t>
-  </si>
-  <si>
-    <t>20k</t>
-  </si>
-  <si>
-    <t>AD7656</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>MCP9700AT</t>
-  </si>
-  <si>
-    <t>HE3621_NO_SPST</t>
-  </si>
-  <si>
-    <t>100R</t>
-  </si>
-  <si>
-    <t>120K</t>
-  </si>
-  <si>
-    <t>22k</t>
-  </si>
-  <si>
-    <t>CON2</t>
-  </si>
-  <si>
-    <t>AD817</t>
-  </si>
-  <si>
-    <t>AD5640</t>
-  </si>
-  <si>
-    <t>TLV341</t>
-  </si>
-  <si>
-    <t>Part Reference</t>
-  </si>
-  <si>
-    <t>U20</t>
-  </si>
-  <si>
-    <t>R48</t>
-  </si>
-  <si>
-    <t>R59</t>
-  </si>
-  <si>
-    <t>U21</t>
-  </si>
-  <si>
-    <t>R58</t>
-  </si>
-  <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>U19</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>IC HS USB TO UART/FIFO 48LQFP</t>
-  </si>
-  <si>
-    <t>FIXED IND 100UH 500MA 600 MOHM</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7PF 100V NP0 0603</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 25V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 39K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>SWITCH PUSH SPST-NO 0.025A 50V</t>
-  </si>
-  <si>
-    <t>RES SMD 12K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>IC EEPROM 2KBIT 2MHZ SOT23-6</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 2K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>CONN RCPT MICRO USB B PCB VERT</t>
-  </si>
-  <si>
-    <t>RES SMD 0.0 OHM JUMPER 1/10W</t>
-  </si>
-  <si>
-    <t>TVS DIODE 24VWM 150VC 0603</t>
-  </si>
-  <si>
-    <t>CRYSTAL 12MHZ 18PF SMD</t>
-  </si>
-  <si>
-    <t>CAP CER 18PF 50V 1% NP0 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 549 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>LED RED RECT CLEAR 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 220 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>CRYSTAL 16MHZ 18PF SMD</t>
-  </si>
-  <si>
-    <t>CAP CER 2.2PF 50V NP0 0603</t>
-  </si>
-  <si>
-    <t>IC MCU ARM M4 32BIT RISC 100LQFP</t>
-  </si>
-  <si>
-    <t>CONN RCPT 20POS VERT DL 2.54MM</t>
-  </si>
-  <si>
-    <t>IC COMPARATOR DUAL 8VSSOP</t>
-  </si>
-  <si>
-    <t>IC OPAMP DIFF 550KHZ RRO 14SOIC</t>
-  </si>
-  <si>
-    <t>CONN BNC JACK STR 50 OHM PCB</t>
-  </si>
-  <si>
-    <t>OPTOISO 3.75KV PHVOLT 8-FLATPACK</t>
-  </si>
-  <si>
-    <t>RES SMD 499 OHM 0.02% 1/4W 0805</t>
-  </si>
-  <si>
-    <t>IC OPAMP GP 6.5MHZ 8DIP</t>
-  </si>
-  <si>
-    <t>RES SMD 50K OHM 0.02% 1/4W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD 20K OHM 0.02% 1/4W 0805</t>
-  </si>
-  <si>
-    <t>IC ADC 16BIT 6CH 250KSPS 64-LQFP</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 25V 20% X5R 0603</t>
-  </si>
-  <si>
-    <t>IC SENSOR THERMAL 2.3V SOT-23-3</t>
-  </si>
-  <si>
-    <t>RELAY REED SPST 500MA 5V</t>
-  </si>
-  <si>
-    <t>RES SMD 100 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 120K OHM 0.1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RES SMD 22K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>SOCKET 4.2 MM SOLDER TAIL SINGLE</t>
-  </si>
-  <si>
-    <t>IC OPAMP GP 50MHZ 8SOIC</t>
-  </si>
-  <si>
-    <t>IC DAC 14BIT SPI/SRL SOT23-8</t>
-  </si>
-  <si>
-    <t>IC OPAMP GP 2.3MHZ RRO SOT23-6</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/FT232HL-REEL/768-1101-1-ND/2614632</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv405=19&amp;FV=fff40002%2Cfff8000b%2Cfffc01ea%2C1c0002%2C3400af%2C380002%2C380004%2C380009%2C380014%2C380016%2C380020%2C400005%2C400006%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv13=40&amp;FV=fff40002%2Cfff8000b%2Cfffc01bd%2Cc0003%2C1c0002%2C1c0003%2C380014%2C400005%2C440005%2C11401c5%2C6540013&amp;k=CERAMIC+CAPACITOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=CKN4080-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv1=1029&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=93LC56BT-I%2FOT&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv1=380&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/ZX80-B-5P/H11890-ND/2469055</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C40400%2C400005&amp;k=chip+resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/PGB1010603MR/F2594CT-ND/813072</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv16=319&amp;FV=fff4000d%2Cfff8016d%2Cfffc0377%2C1c0002%2C1c0003%2C1140003%2C22c019d%2C3f40008%2C8640004%2Cb5005c0&amp;k=CRYSTAL&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?v=490&amp;FV=fff40002%2Cfff8000b%2Cc0001%2C1c0002%2C340067%2C380020%2C400005%2C440012%2C11401c5&amp;k=CERAMIC+CAPACITOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv1=593&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv1=310&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv35=10&amp;FV=fff4000d%2Cfff8016d%2Cfffc0377%2C1c0002%2C1c0003%2C40013f%2C40275f%2C4032ba%2C1140003%2C22c0011%2C3f40008%2C8640004&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?v=490&amp;FV=fff40002%2Cfff8000b%2C1c0002%2C34006f%2C380020%2C400005%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv155=200&amp;FV=fff40027%2Cfff800cd%2C400457&amp;k=STM32F401&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/0901512220/WM8630-ND/3044751</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=fff40027%2Cfff8013d%2C1c0001%2C1c0002%2C1c0006%2Ca4000f%2Ca4006a%2Ca4006d%2Ca40141%2Ca40161%2Ca40168%2Ca4017b%2Ca4018a%2C1140003%2C1a40002%2C3f00002%2C3f00019%2C3f0001a%2C3f0001b%2C3f0001d%2C15100028%2C15100032%2C15100074%2C15100075%2C1510007c%2C15100087%2C15100096%2C151000a9%2C151000b0%2C151000b2%2C151000b4%2C151000cd%2C151000d0%2C182400ab%2C18580016%2C18580054%2C185c0020%2C185c0047%2C185c004b%2C185c0076%2C18680016%2C18680018&amp;k=comparator&amp;mnonly</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/AD8277ARZ-RL/AD8277ARZ-RLCT-ND/4908128</t>
   </si>
   <si>
@@ -720,33 +741,18 @@
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;pv69=3&amp;k=loc111&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=fff40001%2Cfff800e9%2C40226%2Cc007b%2C44006c%2C142c040d&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=fff40001%2Cfff800e9%2C4023e%2Cc007b%2C142c040d&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/PLTT0805Z2002QGT5/PLTT20.0KACT-ND/2552078</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/AD7656BSTZ-REEL/AD7656BSTZ-REELCT-ND/4907889</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?v=445&amp;FV=fff40002%2Cfff8000b%2C1c0002%2C340045%2C380014%2C400005%2C440005%2C440012%2C440013%2C11401c5%2C3f00011%2C3f00019%2C3f0001d%2C3f00027%2C3f00028%2C3f0002a%2C3f0003f%2C6540013%2C654006c%2C6540562%2C6540564%2C6540566%2C6540568%2C65405e6%2C654077f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-search/en?pv1291=88&amp;FV=1c0002&amp;k=MCP9700AT&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=ERJ-3EKF1000V&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv1291=2471&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C4008e%2C80004%2Cc002c%2C1c0002%2C400006%2C400007%2C400008&amp;k=chip+resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv1=320&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/310-87-102-41-001101/1212-1089-ND/3757339</t>
   </si>
   <si>
@@ -759,154 +765,148 @@
     <t>http://www.digikey.com/product-detail/en/TLV341AIDBVR/296-17680-1-ND/716532</t>
   </si>
   <si>
-    <t>Part Type</t>
-  </si>
-  <si>
-    <t>USB COM</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>EEPROM</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>MCU</t>
-  </si>
-  <si>
-    <t>Op Amp</t>
-  </si>
-  <si>
-    <t>Optocoupler</t>
-  </si>
-  <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>Temperature Sensor</t>
-  </si>
-  <si>
-    <t>DAC</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>Push Button</t>
-  </si>
-  <si>
-    <t>TVS</t>
-  </si>
-  <si>
-    <t>Diff Amp</t>
-  </si>
-  <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 25V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv314=3313&amp;FV=fff40003%2Cfff80013%2C1c0002%2C1c0003%2C108002f%2C1400008&amp;k=INDUCTOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=27</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv13=253&amp;FV=fff40002%2Cfff8000b%2Cfffc01bd%2Cc0003%2C1c0002%2C1c0003%2C380014%2C400005%2C440005%2C11401c5%2C6540013&amp;k=CERAMIC+CAPACITOR&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/OPA602BP/OPA602BP-ND/301317</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv1=112&amp;FV=fff40001%2Cfff800e9%2Cfffc000a%2C80002%2Cc0001%2C1c0002%2C400005%2C440067&amp;k=resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=49</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=LTST-C193KRKT-5A&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=26</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-search/en?pv1413=50&amp;FV=141988&amp;k=HE3621&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=32</t>
-  </si>
-  <si>
     <t>J3, J4, J5, J7</t>
   </si>
   <si>
+    <t>U5, U6, U7</t>
+  </si>
+  <si>
+    <t>U16, U18</t>
+  </si>
+  <si>
+    <t>C11, C13, C21, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44, C46, C48, C50, C7, C9</t>
+  </si>
+  <si>
+    <t>C10, C12, C14, C15, C16, C17, C18, C19, C20, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C49, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C62, C63, C64, C65, C70, C71, C72, C73, C74, C75, C76, C8, C80, C82, C86, C88, C90, C92, C93, C94, C95, C96</t>
+  </si>
+  <si>
+    <t>C77, C78, C79, C81</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>R10, R11, R12, R13, R14, R15, R16, R3, R4, R9</t>
+  </si>
+  <si>
+    <t>R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R32, R36, R40, R42, R43, R44, R45, R46, R47, R55, R56, R57, R8</t>
+  </si>
+  <si>
+    <t>R50, R51</t>
+  </si>
+  <si>
+    <t>R5, R6, R7</t>
+  </si>
+  <si>
+    <t>R41, R60</t>
+  </si>
+  <si>
+    <t>R33, R37, R52, R53, R54</t>
+  </si>
+  <si>
+    <t>C66, C67, C83, C84</t>
+  </si>
+  <si>
+    <t>C68, C69</t>
+  </si>
+  <si>
+    <t>C85, C87, C89, C91</t>
+  </si>
+  <si>
+    <t>LS1, LS2, LS3, LS4, LS5, LS6, LS7, LS8</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>D1, D10, D2, D3, D4, D5, D6, D7, D8, D9</t>
+  </si>
+  <si>
+    <t>U10, U11, U13, U14, U15</t>
+  </si>
+  <si>
+    <t>CR1, CR2</t>
+  </si>
+  <si>
+    <t>L1, L2, L3, R49</t>
+  </si>
+  <si>
+    <t>U17A, U17B</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/OPA602BP/OPA602BP-ND/301315</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=887-1053-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=887-1059-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=445-9015-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=445-1316-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=445-5956-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P120KBCCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P10.0KHCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P12.0KHCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P2.00KHCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P220HCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P22.0KHCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P549HCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P0.0GCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=490-9716-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=490-9668-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=490-6392-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=HE207-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=160-1830-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=PLTT499ACT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=PLTT50.0KACT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=SDS850R-104M&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=497-14048-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=296-37236-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
     <t>R34, R35, R38, R39</t>
-  </si>
-  <si>
-    <t>U5, U6, U7</t>
-  </si>
-  <si>
-    <t>U16, U18</t>
-  </si>
-  <si>
-    <t>C11, C13, C21, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44, C46, C48, C50, C7, C9</t>
-  </si>
-  <si>
-    <t>C10, C12, C14, C15, C16, C17, C18, C19, C20, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C49, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C62, C63, C64, C65, C70, C71, C72, C73, C74, C75, C76, C8, C80, C82, C86, C88, C90, C92, C93, C94, C95, C96</t>
-  </si>
-  <si>
-    <t>C77, C78, C79, C81</t>
-  </si>
-  <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
-    <t>R10, R11, R12, R13, R14, R15, R16, R3, R4, R9</t>
-  </si>
-  <si>
-    <t>R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R32, R36, R40, R42, R43, R44, R45, R46, R47, R55, R56, R57, R8</t>
-  </si>
-  <si>
-    <t>R50, R51</t>
-  </si>
-  <si>
-    <t>R5, R6, R7</t>
-  </si>
-  <si>
-    <t>R41, R60</t>
-  </si>
-  <si>
-    <t>R33, R37, R52, R53, R54</t>
-  </si>
-  <si>
-    <t>C66, C67, C83, C84</t>
-  </si>
-  <si>
-    <t>C68, C69</t>
-  </si>
-  <si>
-    <t>C85, C87, C89, C91</t>
-  </si>
-  <si>
-    <t>LS1, LS2, LS3, LS4, LS5, LS6, LS7, LS8</t>
-  </si>
-  <si>
-    <t>SW1, SW2</t>
-  </si>
-  <si>
-    <t>D1, D10, D2, D3, D4, D5, D6, D7, D8, D9</t>
-  </si>
-  <si>
-    <t>U10, U11, U13, U14, U15</t>
-  </si>
-  <si>
-    <t>CR1, CR2</t>
-  </si>
-  <si>
-    <t>L1, L2, L3, R49</t>
-  </si>
-  <si>
-    <t>U17A, U17B</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1282,7 @@
     <col min="8" max="8" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="162.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="2"/>
@@ -1293,34 +1293,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>247</v>
+        <v>105</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1328,34 +1328,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="H2" s="2">
         <v>0.1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1363,34 +1363,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="H3" s="2">
         <v>0.89</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
+        <v>221</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>238</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1398,34 +1398,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="H4" s="2">
         <v>0.16</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>204</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>223</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1433,34 +1433,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="H5" s="2">
         <v>0.1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>227</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1468,34 +1468,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>259</v>
+        <v>81</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>266</v>
+        <v>163</v>
       </c>
       <c r="H6" s="2">
         <v>0.24</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>11</v>
+        <v>195</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1503,34 +1503,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="H7" s="2">
         <v>0.24</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>213</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1538,34 +1538,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>263</v>
+        <v>113</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="H8" s="2">
         <v>0.67</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>18</v>
+        <v>202</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1573,34 +1573,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="H9" s="2">
         <v>0.43</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1611,31 +1611,31 @@
         <v>731315013</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>251</v>
+        <v>112</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="H10" s="2">
         <v>2.56</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>30</v>
+        <v>214</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1643,34 +1643,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>251</v>
+        <v>112</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="H11" s="2">
         <v>0.22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>43</v>
+        <v>227</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1681,31 +1681,31 @@
         <v>901512220</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>251</v>
+        <v>112</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="H12" s="2">
         <v>5.89</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>27</v>
+        <v>211</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1713,34 +1713,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>251</v>
+        <v>112</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="H13" s="2">
         <v>1.39</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1748,34 +1748,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>260</v>
+        <v>107</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="H14" s="2">
         <v>2.48</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>267</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1783,34 +1783,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="H15" s="2">
         <v>2.16</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1818,34 +1818,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="H16" s="2">
         <v>0.94</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>41</v>
+        <v>225</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1853,34 +1853,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="H17" s="2">
         <v>0.1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1888,34 +1888,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="H18" s="2">
         <v>0.1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>14</v>
+        <v>198</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1923,34 +1923,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="H19" s="2">
         <v>11.25</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>34</v>
+        <v>218</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>235</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1958,34 +1958,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="H20" s="2">
         <v>11.25</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>32</v>
+        <v>216</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>234</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1993,34 +1993,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="H21" s="2">
         <v>11.25</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>35</v>
+        <v>219</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2028,34 +2028,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="H22" s="2">
         <v>0.1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>17</v>
+        <v>201</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>220</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2063,34 +2063,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2098,34 +2098,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="H24" s="2">
         <v>0.1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>224</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2133,34 +2133,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="H25" s="2">
         <v>0.1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2168,34 +2168,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="H26" s="2">
         <v>0.1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>42</v>
+        <v>226</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>242</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2203,34 +2203,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="H27" s="2">
         <v>0.1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>23</v>
+        <v>207</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>225</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2238,34 +2238,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="H28" s="2">
         <v>0.1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>15</v>
+        <v>199</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>218</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2273,34 +2273,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="H29" s="2">
         <v>0.1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>216</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2308,34 +2308,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>262</v>
+        <v>110</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="H30" s="2">
         <v>1.51</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>10</v>
+        <v>194</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2343,34 +2343,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>254</v>
+        <v>116</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="H31" s="2">
         <v>13.2</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>33</v>
+        <v>217</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2378,34 +2378,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>255</v>
+        <v>118</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="H32" s="2">
         <v>3.34</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>31</v>
+        <v>215</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2413,34 +2413,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>264</v>
+        <v>117</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>29</v>
+        <v>213</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2448,34 +2448,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>254</v>
+        <v>116</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="H34" s="2">
         <v>1.75</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>28</v>
+        <v>212</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>230</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2483,34 +2483,34 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>253</v>
+        <v>115</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="H35" s="2">
         <v>7.35</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>228</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2518,34 +2518,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>248</v>
+        <v>106</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="H36" s="2">
         <v>4.25</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2553,34 +2553,34 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="H37" s="2">
         <v>0.27</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2588,34 +2588,34 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>258</v>
+        <v>122</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="H38" s="2">
         <v>7.13</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>45</v>
+        <v>229</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2623,34 +2623,34 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>254</v>
+        <v>116</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="H39" s="2">
         <v>1.1599999999999999</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2658,34 +2658,34 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>254</v>
+        <v>116</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="H40" s="2">
         <v>4.92</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>44</v>
+        <v>228</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2693,34 +2693,34 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="G41" s="2" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="H41" s="2">
         <v>0.37</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>38</v>
+        <v>222</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2728,34 +2728,34 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>256</v>
+        <v>119</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>36</v>
+        <v>220</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2763,34 +2763,34 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>252</v>
+        <v>114</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="H43" s="2">
         <v>0.44</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>24</v>
+        <v>208</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2798,34 +2798,34 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>252</v>
+        <v>114</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="H44" s="2">
         <v>0.44</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated discharge resistors, capacitors, and relays.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="327">
   <si>
     <t>Number</t>
   </si>
@@ -129,12 +129,6 @@
     <t>ERJ-3EKF1000V</t>
   </si>
   <si>
-    <t>ERA-8AEB124V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2202V</t>
-  </si>
-  <si>
     <t>310-87-102-41-001101</t>
   </si>
   <si>
@@ -315,12 +309,6 @@
     <t>100R</t>
   </si>
   <si>
-    <t>120K</t>
-  </si>
-  <si>
-    <t>22k</t>
-  </si>
-  <si>
     <t>CON2</t>
   </si>
   <si>
@@ -558,12 +546,6 @@
     <t>RES SMD 100 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 120K OHM 0.1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RES SMD 22K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
     <t>SOCKET 4.2 MM SOLDER TAIL SINGLE</t>
   </si>
   <si>
@@ -693,12 +675,6 @@
     <t>P100HCT-ND</t>
   </si>
   <si>
-    <t>P120KBCCT-ND</t>
-  </si>
-  <si>
-    <t>P22.0KHCT-ND</t>
-  </si>
-  <si>
     <t>1212-1089-ND</t>
   </si>
   <si>
@@ -777,27 +753,15 @@
     <t>C11, C13, C21, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44, C46, C48, C50, C7, C9</t>
   </si>
   <si>
-    <t>C10, C12, C14, C15, C16, C17, C18, C19, C20, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C49, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C62, C63, C64, C65, C70, C71, C72, C73, C74, C75, C76, C8, C80, C82, C86, C88, C90, C92, C93, C94, C95, C96</t>
-  </si>
-  <si>
     <t>C77, C78, C79, C81</t>
   </si>
   <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
-    <t>R10, R11, R12, R13, R14, R15, R16, R3, R4, R9</t>
-  </si>
-  <si>
     <t>R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R32, R36, R40, R42, R43, R44, R45, R46, R47, R55, R56, R57, R8</t>
   </si>
   <si>
     <t>R50, R51</t>
   </si>
   <si>
-    <t>R5, R6, R7</t>
-  </si>
-  <si>
     <t>R41, R60</t>
   </si>
   <si>
@@ -813,15 +777,9 @@
     <t>C85, C87, C89, C91</t>
   </si>
   <si>
-    <t>LS1, LS2, LS3, LS4, LS5, LS6, LS7, LS8</t>
-  </si>
-  <si>
     <t>SW1, SW2</t>
   </si>
   <si>
-    <t>D1, D10, D2, D3, D4, D5, D6, D7, D8, D9</t>
-  </si>
-  <si>
     <t>U10, U11, U13, U14, U15</t>
   </si>
   <si>
@@ -852,9 +810,6 @@
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=445-5956-1-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P120KBCCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P10.0KHCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
   </si>
   <si>
@@ -867,9 +822,6 @@
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P220HCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P22.0KHCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-search/en?pv7=2&amp;k=P549HCT-ND&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
   </si>
   <si>
@@ -907,6 +859,144 @@
   </si>
   <si>
     <t>R34, R35, R38, R39</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>RNX1251K10FKEL</t>
+  </si>
+  <si>
+    <t>RNX200130KFKEL</t>
+  </si>
+  <si>
+    <t>RCL12254R70JNEG</t>
+  </si>
+  <si>
+    <t>CGA3E2X7R1H332K080AA</t>
+  </si>
+  <si>
+    <t>CRCW12064M99FKEA</t>
+  </si>
+  <si>
+    <t>MCA1206MD4991DP500</t>
+  </si>
+  <si>
+    <t>RNX12510M0FKEL</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>1.1k</t>
+  </si>
+  <si>
+    <t>130k</t>
+  </si>
+  <si>
+    <t>3.3nF</t>
+  </si>
+  <si>
+    <t>4.99M</t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>10M</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>RES 1.10K OHM 1% 100 PPM 3W</t>
+  </si>
+  <si>
+    <t>RES 130K OHM 1% 100 PPM 5W</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7 OHM 5% 2W 1225</t>
+  </si>
+  <si>
+    <t>CAP CER 3300PF 50V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 4.99M OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RES SMD 4.99K OHM 0.5% 0.4W 1206</t>
+  </si>
+  <si>
+    <t>RES 10.0M OHM 1% 100 PPM 3W</t>
+  </si>
+  <si>
+    <t>RNX1.10KP-ND</t>
+  </si>
+  <si>
+    <t>RNX130KS-ND</t>
+  </si>
+  <si>
+    <t>RCL4.7FCT-ND</t>
+  </si>
+  <si>
+    <t>445-6921-1-ND</t>
+  </si>
+  <si>
+    <t>541-4.99MFCT-ND</t>
+  </si>
+  <si>
+    <t>MCA1206-4.99K-MDCT-ND</t>
+  </si>
+  <si>
+    <t>RNX10.0MP-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RNX1251K10FKEL/RNX1.10KP-ND/2712917</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RNX200130KFKEL/RNX130KS-ND/2712922</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=fff40001%2Cfff800e9%2Cfffc021d%2C40428%2C80007%2C2b80014%2C2b80016%2C2b80017%2C2b8001c&amp;k=chip+resistor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv14=32&amp;FV=fff40002%2Cfff8000b%2Cfffc01bd%2Cc0002%2Cc0003%2C1c0002%2C34009c%2C380002%2C380009%2C380014%2C380020%2C400005%2C440005%2C11401c5&amp;k=ceramic+capacitor&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?pv7=2&amp;FV=ffec48b8%2Cfff40001%2Cfff800e9%2C40373%2C400007%2C440067%2C44006f&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=30</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MCA1206MD4991DP500/MCA1206-4.99K-MDCT-ND/3883941</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RNX12510M0FKEL/RNX10.0MP-ND/2712919</t>
+  </si>
+  <si>
+    <t>C10, C12, C14, C18, C19, C20, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C49, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C62, C63, C64, C65, C70, C71, C72, C73, C74, C75, C76, C8, C80, C82, C86, C88, C90, C92, C93, C94, C95, C96</t>
+  </si>
+  <si>
+    <t>C15, C16, C17</t>
+  </si>
+  <si>
+    <t>R10, R11, R12, R13, R14, R15, R16, R62, R9</t>
+  </si>
+  <si>
+    <t>LS1, LS10, LS11, LS4, LS5, LS6, LS7, LS8, LS9</t>
+  </si>
+  <si>
+    <t>D1, D10, D11, D2, D3, D4, D5, D6, D7, D8, D9</t>
   </si>
 </sst>
 </file>
@@ -1266,23 +1356,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="162.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="2"/>
@@ -1296,31 +1386,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1331,31 +1421,31 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>253</v>
+        <v>322</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H2" s="2">
         <v>0.1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1366,31 +1456,31 @@
         <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H3" s="2">
         <v>0.89</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1398,34 +1488,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>286</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>293</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>262</v>
+        <v>323</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>158</v>
+        <v>304</v>
       </c>
       <c r="H4" s="2">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>204</v>
+        <v>311</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>286</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1433,34 +1523,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="H5" s="2">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1468,34 +1558,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H6" s="2">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1503,34 +1593,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="H7" s="2">
         <v>0.24</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1538,34 +1628,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H8" s="2">
-        <v>0.67</v>
+        <v>0.24</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1573,136 +1663,136 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H9" s="2">
-        <v>0.43</v>
+        <v>0.67</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>731315013</v>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>249</v>
+        <v>326</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="H10" s="2">
-        <v>2.56</v>
+        <v>0.43</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>239</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
+      <c r="B11" s="2">
+        <v>731315013</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>140</v>
+        <v>241</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="H11" s="2">
-        <v>0.22</v>
+        <v>2.56</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>901512220</v>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="H12" s="2">
-        <v>5.89</v>
+        <v>0.22</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>237</v>
@@ -1712,35 +1802,35 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
+      <c r="B13" s="2">
+        <v>901512220</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>129</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H13" s="2">
-        <v>1.39</v>
+        <v>5.89</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1748,34 +1838,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>270</v>
+        <v>125</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="H14" s="2">
-        <v>2.48</v>
+        <v>1.39</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>293</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1783,69 +1873,69 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="H15" s="2">
-        <v>2.16</v>
+        <v>2.48</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>223</v>
+        <v>3</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>255</v>
+        <v>325</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H16" s="2">
-        <v>0.94</v>
+        <v>2.16</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1856,31 +1946,31 @@
         <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>256</v>
+        <v>324</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H17" s="2">
         <v>0.1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1891,31 +1981,31 @@
         <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H18" s="2">
         <v>0.1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1923,34 +2013,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>284</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>60</v>
+        <v>290</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>92</v>
+        <v>292</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>136</v>
+        <v>281</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>173</v>
+        <v>302</v>
       </c>
       <c r="H19" s="2">
-        <v>11.25</v>
+        <v>6.4</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>218</v>
+        <v>309</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1958,34 +2048,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H20" s="2">
         <v>11.25</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1993,34 +2083,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>283</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>290</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>137</v>
+        <v>282</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>174</v>
+        <v>301</v>
       </c>
       <c r="H21" s="2">
-        <v>11.25</v>
+        <v>6.4</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>241</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2028,34 +2118,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>261</v>
+        <v>131</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="H22" s="2">
-        <v>0.1</v>
+        <v>11.25</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2063,34 +2153,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>296</v>
+        <v>133</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>25</v>
+        <v>170</v>
+      </c>
+      <c r="H23" s="2">
+        <v>11.25</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>25</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2098,34 +2188,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H24" s="2">
         <v>0.1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2133,31 +2223,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.1</v>
+        <v>25</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>188</v>
+        <v>25</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>193</v>
+        <v>25</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>25</v>
@@ -2168,34 +2258,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="H26" s="2">
         <v>0.1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2203,34 +2293,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>258</v>
+        <v>121</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H27" s="2">
         <v>0.1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>282</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2238,34 +2328,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>12</v>
+        <v>287</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>294</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>128</v>
+        <v>298</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>153</v>
+        <v>305</v>
       </c>
       <c r="H28" s="2">
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>199</v>
+        <v>312</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2273,34 +2363,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>126</v>
+        <v>247</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="H29" s="2">
         <v>0.1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2308,34 +2398,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>266</v>
+        <v>124</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>149</v>
       </c>
       <c r="H30" s="2">
-        <v>1.51</v>
+        <v>0.1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2343,34 +2433,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>268</v>
+        <v>122</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="H31" s="2">
-        <v>13.2</v>
+        <v>0.1</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2378,34 +2468,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>27</v>
+        <v>288</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>89</v>
+        <v>295</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>134</v>
+        <v>299</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>170</v>
+        <v>306</v>
       </c>
       <c r="H32" s="2">
-        <v>3.34</v>
+        <v>0.63</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>215</v>
+        <v>313</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>240</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2413,34 +2503,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>26</v>
+        <v>289</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>58</v>
+        <v>290</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>87</v>
+        <v>296</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>251</v>
+        <v>300</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>25</v>
+        <v>307</v>
+      </c>
+      <c r="H33" s="2">
+        <v>6.4</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>213</v>
+        <v>314</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2448,34 +2538,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>24</v>
+        <v>285</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>85</v>
+        <v>58</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>167</v>
+        <v>303</v>
       </c>
       <c r="H34" s="2">
-        <v>1.75</v>
+        <v>7.23</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>212</v>
+        <v>310</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2483,34 +2573,34 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>132</v>
+        <v>253</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="H35" s="2">
-        <v>7.35</v>
+        <v>1.51</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="K35" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2518,34 +2608,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>124</v>
+        <v>254</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="H36" s="2">
-        <v>4.25</v>
+        <v>13.2</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2553,34 +2643,34 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="H37" s="2">
-        <v>0.27</v>
+        <v>3.34</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2588,34 +2678,34 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>141</v>
+        <v>243</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H38" s="2">
-        <v>7.13</v>
+        <v>164</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2623,34 +2713,34 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>142</v>
+        <v>257</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="H39" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.75</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2658,34 +2748,34 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="H40" s="2">
-        <v>4.92</v>
+        <v>7.35</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2693,34 +2783,34 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="G41" s="2" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="H41" s="2">
-        <v>0.37</v>
+        <v>4.25</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2728,34 +2818,34 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>25</v>
+        <v>147</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.27</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2763,34 +2853,34 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="H43" s="2">
-        <v>0.44</v>
+        <v>7.13</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2798,38 +2888,198 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H45" s="2">
+        <v>4.92</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H44" s="2">
+      <c r="C49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H49" s="2">
         <v>0.44</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>273</v>
+      <c r="I49" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K44">
+  <sortState ref="A2:K49">
     <sortCondition ref="F2:F44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added gnd to DAC removed bypass caps for dc_bias.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
@@ -850,10 +850,10 @@
     <t>U6, U7</t>
   </si>
   <si>
-    <t>C1, C3, C5, C7, C17, C18, C20, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44, C46</t>
-  </si>
-  <si>
-    <t>C2, C4, C6, C8, C12, C13, C14, C15, C16, C19, C21, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C66, C67, C68, C69, C70, C71, C72, C75, C76, C77, C78, C80, C81, C83, C87, C89, C91, C93, C94, C95, C96, C97</t>
+    <t>C1, C3, C5, C17, C18, C20, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44, C46</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C12, C13, C14, C15, C16, C19, C21, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C66, C67, C68, C69, C70, C71, C72, C75, C76, C77, C78, C80, C81, C83, C87, C89, C91, C93, C94, C95, C96, C97</t>
   </si>
   <si>
     <t>C73, C74, C79, C82</t>
@@ -871,7 +871,7 @@
     <t>C86, C88, C90, C92</t>
   </si>
   <si>
-    <t>J1, J3</t>
+    <t>J1, J3, J8</t>
   </si>
   <si>
     <t>J6, J7</t>
@@ -1763,11 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,7 +1907,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>278</v>
@@ -1943,7 +1942,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>279</v>
@@ -2153,7 +2152,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>285</v>
@@ -3619,10 +3618,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:J218">
+  <sortState ref="B2:J217">
     <sortCondition ref="E2:E500"/>
     <sortCondition ref="B2:B500"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reannotated schematic after removing 2 caps.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="720" yWindow="330" windowWidth="22755" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="CAPMEASCIRCUIT" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
     <t>CON2</t>
   </si>
   <si>
-    <t>J2</t>
+    <t>J3</t>
   </si>
   <si>
     <t>SOCKET 4.2 MM SOLDER TAIL SINGLE</t>
@@ -181,7 +181,7 @@
     <t>JTAG</t>
   </si>
   <si>
-    <t>J4</t>
+    <t>J5</t>
   </si>
   <si>
     <t>CONN RCPT 20POS VERT DL 2.54MM</t>
@@ -199,7 +199,7 @@
     <t>USB-MICRO-B</t>
   </si>
   <si>
-    <t>J5</t>
+    <t>J6</t>
   </si>
   <si>
     <t>CONN RCPT MICRO USB B PCB VERT</t>
@@ -214,7 +214,7 @@
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>COM2</t>
+    <t>COM1</t>
   </si>
   <si>
     <t>DB9 Connector</t>
@@ -850,31 +850,31 @@
     <t>U6, U7</t>
   </si>
   <si>
-    <t>C1, C3, C5, C17, C18, C20, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44, C46</t>
-  </si>
-  <si>
-    <t>C2, C4, C6, C12, C13, C14, C15, C16, C19, C21, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C60, C61, C66, C67, C68, C69, C70, C71, C72, C75, C76, C77, C78, C80, C81, C83, C87, C89, C91, C93, C94, C95, C96, C97</t>
-  </si>
-  <si>
-    <t>C73, C74, C79, C82</t>
-  </si>
-  <si>
-    <t>C9, C10, C11</t>
-  </si>
-  <si>
-    <t>C62, C63, C84, C85</t>
-  </si>
-  <si>
-    <t>C64, C65</t>
-  </si>
-  <si>
-    <t>C86, C88, C90, C92</t>
-  </si>
-  <si>
-    <t>J1, J3, J8</t>
-  </si>
-  <si>
-    <t>J6, J7</t>
+    <t>C1, C3, C5, C15, C16, C18, C20, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C10, C11, C12, C13, C14, C17, C19, C21, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C46, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C64, C65, C66, C67, C68, C69, C70, C73, C74, C75, C76, C78, C79, C81, C85, C87, C89, C91, C92, C93, C94, C95</t>
+  </si>
+  <si>
+    <t>C71, C72, C77, C80</t>
+  </si>
+  <si>
+    <t>C7, C8, C9</t>
+  </si>
+  <si>
+    <t>C60, C61, C82, C83</t>
+  </si>
+  <si>
+    <t>C62, C63</t>
+  </si>
+  <si>
+    <t>C84, C86, C88, C90</t>
+  </si>
+  <si>
+    <t>J1, J2, J4</t>
+  </si>
+  <si>
+    <t>J7, J8</t>
   </si>
   <si>
     <t>U16, U18</t>
@@ -907,13 +907,13 @@
     <t>R8, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R33, R37, R42, R43, R44, R45, R46, R47, R48, R50, R56, R57, R58</t>
   </si>
   <si>
-    <t>R51, R53</t>
+    <t>R51, R52</t>
   </si>
   <si>
     <t>R41, R61</t>
   </si>
   <si>
-    <t>R34, R38, R52, R54, R55</t>
+    <t>R34, R38, R53, R54, R55</t>
   </si>
   <si>
     <t>R3, R4</t>
@@ -1763,11 +1763,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3571,54 +3569,44 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>51</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="F52" s="2">
         <v>1</v>
       </c>
-      <c r="G52" s="4" t="s">
+    </row>
+    <row r="215" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D215" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G215" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>52</v>
-      </c>
-      <c r="D53" s="2" t="s">
+    <row r="217" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D217" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="G217" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>53</v>
-      </c>
-      <c r="D54" s="2" t="s">
+    <row r="221" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D221" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G221" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>54</v>
-      </c>
-      <c r="D55" s="2" t="s">
+    <row r="223" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D223" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G223" s="4" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:J217">
+  <sortState ref="B2:J433">
     <sortCondition ref="E2:E500"/>
     <sortCondition ref="B2:B500"/>
   </sortState>

</xml_diff>

<commit_message>
added sallen-key filter to the output of the current.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="22755" windowHeight="9750"/>
+    <workbookView xWindow="720" yWindow="360" windowWidth="22755" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="CAPMEASCIRCUIT" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="359">
   <si>
     <t>PGB1010603MR</t>
   </si>
@@ -79,6 +79,66 @@
     <t>445-6921-1-ND</t>
   </si>
   <si>
+    <t>CL21C102JBCNNNC</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V 5% NP0 0805</t>
+  </si>
+  <si>
+    <t>1276-1147-1-ND</t>
+  </si>
+  <si>
+    <t>CL21C222JBFNNNE</t>
+  </si>
+  <si>
+    <t>2.2nF</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>CAP CER 2200PF 50V 5% NP0 0805</t>
+  </si>
+  <si>
+    <t>1276-2993-1-ND</t>
+  </si>
+  <si>
+    <t>C2012C0G1H153J085AA</t>
+  </si>
+  <si>
+    <t>15nF</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>CAP CER 0.015UF 50V 5% C0G 0805</t>
+  </si>
+  <si>
+    <t>445-7521-1-ND</t>
+  </si>
+  <si>
+    <t>CL21C911JBCNNNC</t>
+  </si>
+  <si>
+    <t>910pF</t>
+  </si>
+  <si>
+    <t>CAP CER 910PF 50V 5% NP0 0805</t>
+  </si>
+  <si>
+    <t>1276-2698-1-ND</t>
+  </si>
+  <si>
     <t>GRM1885C1H180FA01D</t>
   </si>
   <si>
@@ -214,7 +274,7 @@
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>COM1</t>
+    <t>COM2</t>
   </si>
   <si>
     <t>DB9 Connector</t>
@@ -349,12 +409,114 @@
     <t>RCL4.7FCT-ND</t>
   </si>
   <si>
+    <t>ERJ-3EKF1000V</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>P100HCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF4641V</t>
+  </si>
+  <si>
+    <t>4.64k</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>RES SMD 4.64K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P4.64KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF6491V</t>
+  </si>
+  <si>
+    <t>6.49k</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>RES SMD 6.49K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P6.49KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF2871V</t>
+  </si>
+  <si>
+    <t>2.87k</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>RES SMD 2.87K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P2.87KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF5361V</t>
+  </si>
+  <si>
+    <t>5.36k</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>RES SMD 5.36K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P5.36KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1401V</t>
+  </si>
+  <si>
+    <t>1.4k</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>RES SMD 1.4K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P1.40KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1621V</t>
+  </si>
+  <si>
+    <t>1.62k</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>RES SMD 1.62K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P1.62KCCT-ND</t>
+  </si>
+  <si>
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -364,25 +526,13 @@
     <t>P10.0KHCT-ND</t>
   </si>
   <si>
-    <t>ERJ-3EKF1000V</t>
-  </si>
-  <si>
-    <t>100R</t>
-  </si>
-  <si>
-    <t>RES SMD 100 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>P100HCT-ND</t>
-  </si>
-  <si>
     <t>PLTT0805Z5002QGT5</t>
   </si>
   <si>
     <t>50k</t>
   </si>
   <si>
-    <t>R30</t>
+    <t>R34</t>
   </si>
   <si>
     <t>RES SMD 50K OHM 0.02% 1/4W 0805</t>
@@ -397,7 +547,7 @@
     <t>499R</t>
   </si>
   <si>
-    <t>R31</t>
+    <t>R35</t>
   </si>
   <si>
     <t>RES SMD 499 OHM 0.02% 1/4W 0805</t>
@@ -412,7 +562,7 @@
     <t>20k</t>
   </si>
   <si>
-    <t>R32</t>
+    <t>R36</t>
   </si>
   <si>
     <t>RES SMD 20K OHM 0.02% 1/4W 0805</t>
@@ -436,18 +586,18 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
     <t>R39</t>
   </si>
   <si>
     <t>R40</t>
   </si>
   <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
     <t>ERJ-3EKF5490V</t>
   </si>
   <si>
@@ -466,7 +616,7 @@
     <t>39K</t>
   </si>
   <si>
-    <t>R49</t>
+    <t>R54</t>
   </si>
   <si>
     <t>RES SMD 39K OHM 1% 1/10W 0603</t>
@@ -493,7 +643,7 @@
     <t>2K</t>
   </si>
   <si>
-    <t>R59</t>
+    <t>R64</t>
   </si>
   <si>
     <t>RES SMD 2K OHM 1% 1/10W 0603</t>
@@ -508,7 +658,7 @@
     <t>12k</t>
   </si>
   <si>
-    <t>R60</t>
+    <t>R65</t>
   </si>
   <si>
     <t>RES SMD 12K OHM 1% 1/10W 0603</t>
@@ -589,12 +739,102 @@
     <t>AD817ARZ-REEL7CT-ND</t>
   </si>
   <si>
+    <t>LF356MX/NOPB</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>LF356MX</t>
+  </si>
+  <si>
+    <t>IC OPAMP JFET 5MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>LF356MX/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>AD7656BSTZ-REEL</t>
+  </si>
+  <si>
+    <t>AD7656</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>IC ADC 16BIT 6CH 250KSPS 64-LQFP</t>
+  </si>
+  <si>
+    <t>AD7656BSTZ-REELCT-ND</t>
+  </si>
+  <si>
+    <t>OPA602BP</t>
+  </si>
+  <si>
+    <t>OPA602</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 6.5MHZ 8DIP</t>
+  </si>
+  <si>
+    <t>OPA602BP-ND</t>
+  </si>
+  <si>
+    <t>LOC111PTR</t>
+  </si>
+  <si>
+    <t>IXYS</t>
+  </si>
+  <si>
+    <t>LOC111</t>
+  </si>
+  <si>
+    <t>Optocoupler</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>OPTOISO 3.75KV PHVOLT 8-FLATPACK</t>
+  </si>
+  <si>
+    <t>CLA118CT-ND</t>
+  </si>
+  <si>
+    <t>AD8277ARZ-RL</t>
+  </si>
+  <si>
+    <t>AD8277</t>
+  </si>
+  <si>
+    <t>Diff Amp</t>
+  </si>
+  <si>
+    <t>IC OPAMP DIFF 550KHZ RRO 14SOIC</t>
+  </si>
+  <si>
+    <t>AD8277ARZ-RLCT-ND</t>
+  </si>
+  <si>
+    <t>TLV1702AIDGKR</t>
+  </si>
+  <si>
+    <t>TLV1702</t>
+  </si>
+  <si>
+    <t>IC COMPARATOR DUAL 8VSSOP</t>
+  </si>
+  <si>
+    <t>296-37236-1-ND</t>
+  </si>
+  <si>
     <t>CD74AC244M96</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
     <t>74AC245</t>
   </si>
   <si>
@@ -619,7 +859,7 @@
     <t>Temperature Sensor</t>
   </si>
   <si>
-    <t>U8</t>
+    <t>U20</t>
   </si>
   <si>
     <t>IC SENSOR THERMAL 2.3V SOT-23-3</t>
@@ -628,84 +868,6 @@
     <t>MCP9700AT-E/TTCT-ND</t>
   </si>
   <si>
-    <t>AD7656BSTZ-REEL</t>
-  </si>
-  <si>
-    <t>AD7656</t>
-  </si>
-  <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>IC ADC 16BIT 6CH 250KSPS 64-LQFP</t>
-  </si>
-  <si>
-    <t>AD7656BSTZ-REELCT-ND</t>
-  </si>
-  <si>
-    <t>OPA602BP</t>
-  </si>
-  <si>
-    <t>OPA602</t>
-  </si>
-  <si>
-    <t>IC OPAMP GP 6.5MHZ 8DIP</t>
-  </si>
-  <si>
-    <t>OPA602BP-ND</t>
-  </si>
-  <si>
-    <t>LOC111PTR</t>
-  </si>
-  <si>
-    <t>IXYS</t>
-  </si>
-  <si>
-    <t>LOC111</t>
-  </si>
-  <si>
-    <t>Optocoupler</t>
-  </si>
-  <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>OPTOISO 3.75KV PHVOLT 8-FLATPACK</t>
-  </si>
-  <si>
-    <t>CLA118CT-ND</t>
-  </si>
-  <si>
-    <t>AD8277ARZ-RL</t>
-  </si>
-  <si>
-    <t>AD8277</t>
-  </si>
-  <si>
-    <t>Diff Amp</t>
-  </si>
-  <si>
-    <t>IC OPAMP DIFF 550KHZ RRO 14SOIC</t>
-  </si>
-  <si>
-    <t>AD8277ARZ-RLCT-ND</t>
-  </si>
-  <si>
-    <t>TLV1702AIDGKR</t>
-  </si>
-  <si>
-    <t>TLV1702</t>
-  </si>
-  <si>
-    <t>IC COMPARATOR DUAL 8VSSOP</t>
-  </si>
-  <si>
-    <t>296-37236-1-ND</t>
-  </si>
-  <si>
     <t>STM32F401VCT6</t>
   </si>
   <si>
@@ -718,7 +880,7 @@
     <t>MCU</t>
   </si>
   <si>
-    <t>U19</t>
+    <t>U21</t>
   </si>
   <si>
     <t>IC MCU ARM M4 32BIT RISC 100LQFP</t>
@@ -739,7 +901,7 @@
     <t>USB COM</t>
   </si>
   <si>
-    <t>U20</t>
+    <t>U22</t>
   </si>
   <si>
     <t>IC HS USB TO UART/FIFO 48LQFP</t>
@@ -757,7 +919,7 @@
     <t>RS232 Transceiver</t>
   </si>
   <si>
-    <t>U21</t>
+    <t>U23</t>
   </si>
   <si>
     <t>IC LINE DRVR/RCVR RS232 16-TSSOP</t>
@@ -772,7 +934,7 @@
     <t>EEPROM</t>
   </si>
   <si>
-    <t>U22</t>
+    <t>U24</t>
   </si>
   <si>
     <t>IC EEPROM 2KBIT 2MHZ SOT23-6</t>
@@ -847,28 +1009,31 @@
     <t>Qnty</t>
   </si>
   <si>
-    <t>U6, U7</t>
-  </si>
-  <si>
-    <t>C1, C3, C5, C15, C16, C18, C20, C22, C24, C26, C28, C30, C32, C34, C36, C38, C40, C42, C44</t>
-  </si>
-  <si>
-    <t>C2, C4, C6, C10, C11, C12, C13, C14, C17, C19, C21, C23, C25, C27, C29, C31, C33, C35, C37, C39, C41, C43, C45, C46, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C57, C58, C59, C64, C65, C66, C67, C68, C69, C70, C73, C74, C75, C76, C78, C79, C81, C85, C87, C89, C91, C92, C93, C94, C95</t>
-  </si>
-  <si>
-    <t>C71, C72, C77, C80</t>
+    <t>U18, U19</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C11, C13, C15, C17, C19, C21, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C49, C51, C53, C55, C57, C76</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C10, C12, C14, C16, C18, C20, C22, C30, C32, C34, C36, C38, C40, C42, C44, C46, C48, C50, C52, C54, C56, C58, C59, C60, C61, C62, C63, C64, C65, C66, C67, C68, C69, C70, C71, C72, C73, C74, C75, C81, C82, C83, C84, C85, C86, C87, C90, C91, C92, C93, C95, C96, C98, C102, C104, C106, C108, C109, C110, C111, C112</t>
+  </si>
+  <si>
+    <t>C88, C89, C94, C97</t>
   </si>
   <si>
     <t>C7, C8, C9</t>
   </si>
   <si>
-    <t>C60, C61, C82, C83</t>
-  </si>
-  <si>
-    <t>C62, C63</t>
-  </si>
-  <si>
-    <t>C84, C86, C88, C90</t>
+    <t>C26, C27, C28</t>
+  </si>
+  <si>
+    <t>C77, C78, C99, C100</t>
+  </si>
+  <si>
+    <t>C79, C80</t>
+  </si>
+  <si>
+    <t>C101, C103, C105, C107</t>
   </si>
   <si>
     <t>J1, J2, J4</t>
@@ -877,7 +1042,7 @@
     <t>J7, J8</t>
   </si>
   <si>
-    <t>U16, U18</t>
+    <t>U15, U17</t>
   </si>
   <si>
     <t>L1, L2, L3</t>
@@ -886,13 +1051,16 @@
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
   </si>
   <si>
-    <t>U3, U4, U5</t>
-  </si>
-  <si>
-    <t>U10, U11, U13, U14, U15</t>
-  </si>
-  <si>
-    <t>U17A, U17B</t>
+    <t>U3, U4</t>
+  </si>
+  <si>
+    <t>U5, U6, U7</t>
+  </si>
+  <si>
+    <t>U9, U10, U12, U13, U14</t>
+  </si>
+  <si>
+    <t>U16A, U16B</t>
   </si>
   <si>
     <t>SW1, SW2</t>
@@ -901,19 +1069,19 @@
     <t>LS1, LS2, LS3, LS4, LS5, LS6, LS7, LS8, LS9</t>
   </si>
   <si>
-    <t>R9, R10, R11, R12, R13, R14, R15, R16, R17</t>
-  </si>
-  <si>
-    <t>R8, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R33, R37, R42, R43, R44, R45, R46, R47, R48, R50, R56, R57, R58</t>
-  </si>
-  <si>
-    <t>R51, R52</t>
-  </si>
-  <si>
-    <t>R41, R61</t>
-  </si>
-  <si>
-    <t>R34, R38, R53, R54, R55</t>
+    <t>R8, R9, R10, R11, R12, R13, R14, R15, R16</t>
+  </si>
+  <si>
+    <t>R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R37, R41, R45, R46, R48, R49, R50, R51, R52, R53, R55, R61, R62, R63</t>
+  </si>
+  <si>
+    <t>R56, R58</t>
+  </si>
+  <si>
+    <t>R47, R66</t>
+  </si>
+  <si>
+    <t>R38, R42, R57, R59, R60</t>
   </si>
   <si>
     <t>R3, R4</t>
@@ -1763,7 +1931,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K223"/>
+  <dimension ref="A1:K255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1785,37 +1953,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>358</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>321</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>268</v>
+        <v>322</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>269</v>
+        <v>323</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>270</v>
+        <v>324</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>276</v>
+        <v>330</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>271</v>
+        <v>325</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>272</v>
+        <v>326</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>273</v>
+        <v>327</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>274</v>
+        <v>328</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>275</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1823,25 +1991,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>207</v>
+        <v>249</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="I2" s="2">
         <v>24.28</v>
@@ -1850,7 +2018,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>209</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1858,25 +2026,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>191</v>
+        <v>272</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>192</v>
+        <v>242</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>277</v>
+        <v>331</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>195</v>
+        <v>275</v>
       </c>
       <c r="I3" s="2">
         <v>0.91</v>
@@ -1885,10 +2053,10 @@
         <v>5</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1905,10 +2073,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>278</v>
+        <v>332</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>11</v>
@@ -1923,7 +2091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1940,10 +2108,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>279</v>
+        <v>333</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>15</v>
@@ -1963,13 +2131,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
@@ -1978,10 +2146,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>280</v>
+        <v>334</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="I6" s="2">
         <v>0.24</v>
@@ -1990,7 +2158,7 @@
         <v>5</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1998,34 +2166,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>281</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I7" s="2">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2033,34 +2201,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>282</v>
+        <v>335</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2068,34 +2236,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>283</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2103,104 +2271,104 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>284</v>
+        <v>29</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2">
-        <v>0.24</v>
+        <v>0.17</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>731315013</v>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2">
         <v>3</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I11" s="2">
-        <v>2.56</v>
+        <v>0.1</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>901512220</v>
+      <c r="B12" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="2">
-        <v>5.89</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2208,34 +2376,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="I13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2243,104 +2411,104 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>61</v>
+        <v>339</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I14" s="2">
-        <v>1.39</v>
+        <v>0.24</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>262</v>
+      <c r="B15" s="2">
+        <v>731315013</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>256</v>
+        <v>63</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>263</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>258</v>
+        <v>65</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>264</v>
+        <v>340</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>265</v>
+        <v>66</v>
       </c>
       <c r="I15" s="2">
-        <v>0.44</v>
+        <v>2.56</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>255</v>
+      <c r="B16" s="2">
+        <v>901512220</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>256</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>257</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>258</v>
+        <v>65</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>259</v>
+        <v>75</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>260</v>
+        <v>76</v>
       </c>
       <c r="I16" s="2">
-        <v>0.44</v>
+        <v>5.89</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>261</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2348,34 +2516,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>174</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>175</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>176</v>
+        <v>65</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>177</v>
+        <v>71</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="I17" s="2">
-        <v>7.13</v>
+        <v>0.22</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>179</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2383,34 +2551,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="F18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>286</v>
+        <v>81</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="I18" s="2">
-        <v>3.9</v>
+        <v>1.39</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2418,34 +2586,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>221</v>
+        <v>316</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>174</v>
+        <v>310</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>222</v>
+        <v>317</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>223</v>
+        <v>312</v>
       </c>
       <c r="F19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>224</v>
+        <v>319</v>
       </c>
       <c r="I19" s="2">
-        <v>4.4000000000000004</v>
+        <v>0.44</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>225</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2453,34 +2621,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>198</v>
+        <v>310</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>252</v>
+        <v>313</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>253</v>
+        <v>314</v>
       </c>
       <c r="I20" s="2">
-        <v>0.27</v>
+        <v>0.44</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>254</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2488,34 +2656,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>224</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>77</v>
+        <v>225</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>78</v>
+        <v>226</v>
       </c>
       <c r="F21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>288</v>
+        <v>227</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
       <c r="I21" s="2">
-        <v>2.48</v>
+        <v>7.13</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>75</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2523,34 +2691,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="F22" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>289</v>
+        <v>341</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="I22" s="2">
-        <v>0.43</v>
+        <v>3.9</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2558,34 +2726,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="F23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>234</v>
+        <v>342</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
       <c r="I23" s="2">
-        <v>7.35</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2593,34 +2761,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>187</v>
+        <v>304</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>174</v>
+        <v>278</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>188</v>
+        <v>304</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>183</v>
+        <v>305</v>
       </c>
       <c r="F24" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>189</v>
+        <v>307</v>
       </c>
       <c r="I24" s="2">
-        <v>4.92</v>
+        <v>0.27</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>190</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2628,34 +2796,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>210</v>
+        <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="F25" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>291</v>
+        <v>343</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>212</v>
+        <v>99</v>
       </c>
       <c r="I25" s="2">
-        <v>13.2</v>
+        <v>2.48</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>213</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2663,34 +2831,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>227</v>
+        <v>60</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>183</v>
+        <v>60</v>
       </c>
       <c r="F26" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>292</v>
+        <v>344</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>228</v>
+        <v>61</v>
       </c>
       <c r="I26" s="2">
-        <v>1.75</v>
+        <v>0.43</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>229</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2698,34 +2866,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>181</v>
+        <v>285</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>182</v>
+        <v>286</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>183</v>
+        <v>287</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>184</v>
+        <v>288</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>185</v>
+        <v>289</v>
       </c>
       <c r="I27" s="2">
-        <v>1.1599999999999999</v>
+        <v>7.35</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>186</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2733,34 +2901,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="F28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>218</v>
+        <v>345</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="I28" s="2">
-        <v>3.34</v>
+        <v>4.92</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2768,34 +2936,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>168</v>
+        <v>242</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>169</v>
+        <v>243</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>170</v>
+        <v>233</v>
       </c>
       <c r="F29" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>293</v>
+        <v>346</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
       <c r="I29" s="2">
-        <v>1.51</v>
+        <v>1.01</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>172</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2803,34 +2971,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>252</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1</v>
+        <v>231</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>71</v>
+        <v>253</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>72</v>
+        <v>233</v>
       </c>
       <c r="F30" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>294</v>
+        <v>347</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>73</v>
+        <v>254</v>
       </c>
       <c r="I30" s="2">
-        <v>2.16</v>
+        <v>13.2</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>74</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2838,34 +3006,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>96</v>
+        <v>268</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>97</v>
+        <v>231</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>98</v>
+        <v>269</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>83</v>
+        <v>233</v>
       </c>
       <c r="F31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>99</v>
+        <v>348</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>100</v>
+        <v>270</v>
       </c>
       <c r="I31" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.75</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>101</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2873,69 +3041,69 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>83</v>
+        <v>233</v>
       </c>
       <c r="F32" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>295</v>
+        <v>234</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
       <c r="I32" s="2">
-        <v>0.1</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>113</v>
+        <v>258</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>83</v>
+        <v>259</v>
       </c>
       <c r="F33" s="2">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>296</v>
+        <v>260</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>114</v>
+        <v>261</v>
       </c>
       <c r="I33" s="2">
-        <v>0.1</v>
+        <v>3.34</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>115</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2943,34 +3111,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>112</v>
+        <v>218</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="F34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>164</v>
+        <v>349</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>165</v>
+        <v>221</v>
       </c>
       <c r="I34" s="2">
-        <v>0.1</v>
+        <v>1.51</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2978,34 +3146,34 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>157</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F35" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>159</v>
+        <v>350</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
       </c>
       <c r="I35" s="2">
-        <v>0.1</v>
+        <v>2.16</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>161</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3013,34 +3181,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F36" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>297</v>
+        <v>119</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="I36" s="2">
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3048,25 +3216,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F37" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="I37" s="2">
         <v>0.1</v>
@@ -3075,33 +3243,33 @@
         <v>5</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F38" s="2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>298</v>
+        <v>352</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="I38" s="2">
         <v>0.1</v>
@@ -3110,7 +3278,7 @@
         <v>5</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3118,25 +3286,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>136</v>
+        <v>213</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F39" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>299</v>
+        <v>214</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="I39" s="2">
         <v>0.1</v>
@@ -3145,7 +3313,7 @@
         <v>5</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>138</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3153,34 +3321,34 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>207</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="I40" s="2">
-        <v>0.63</v>
+        <v>0.1</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3188,34 +3356,34 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>130</v>
+        <v>203</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>132</v>
+        <v>353</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="I41" s="2">
-        <v>11.25</v>
+        <v>0.1</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3223,34 +3391,34 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>125</v>
+        <v>198</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>126</v>
+        <v>199</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>128</v>
+        <v>201</v>
       </c>
       <c r="I42" s="2">
-        <v>11.25</v>
+        <v>0.1</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3258,34 +3426,34 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F43" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>122</v>
+        <v>354</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>123</v>
+        <v>196</v>
       </c>
       <c r="I43" s="2">
-        <v>11.25</v>
+        <v>0.1</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3293,34 +3461,34 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="2">
-        <v>4.7</v>
+        <v>132</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F44" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>108</v>
+        <v>355</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="I44" s="2">
-        <v>7.23</v>
+        <v>0.1</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3328,34 +3496,34 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="I45" s="2">
-        <v>6.4</v>
+        <v>0.1</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3363,34 +3531,34 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F46" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>300</v>
+        <v>163</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>94</v>
+        <v>164</v>
       </c>
       <c r="I46" s="2">
-        <v>6.4</v>
+        <v>0.1</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3398,34 +3566,34 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="I47" s="2">
-        <v>6.4</v>
+        <v>0.1</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3433,34 +3601,34 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>244</v>
+        <v>136</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>192</v>
+        <v>132</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>245</v>
+        <v>137</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>246</v>
+        <v>103</v>
       </c>
       <c r="F48" s="2">
         <v>1</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>247</v>
+        <v>138</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>248</v>
+        <v>139</v>
       </c>
       <c r="I48" s="2">
-        <v>2.39</v>
+        <v>0.1</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>249</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3468,34 +3636,34 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>197</v>
+        <v>151</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>198</v>
+        <v>132</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>200</v>
+        <v>103</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="I49" s="2">
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3503,34 +3671,34 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F50" s="2">
         <v>1</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F50" s="2">
-        <v>2</v>
-      </c>
       <c r="G50" s="4" t="s">
-        <v>301</v>
+        <v>143</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
       <c r="I50" s="2">
-        <v>0.67</v>
+        <v>0.1</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3538,75 +3706,455 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>237</v>
+        <v>122</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>238</v>
+        <v>117</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>239</v>
+        <v>123</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>240</v>
+        <v>103</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>241</v>
+        <v>124</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>242</v>
+        <v>125</v>
       </c>
       <c r="I51" s="2">
-        <v>4.25</v>
+        <v>0.63</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>243</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="F52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D215" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G215" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="217" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D217" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G217" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="221" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D221" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G221" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="223" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D223" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G223" s="4" t="s">
-        <v>143</v>
+      <c r="G52" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I52" s="2">
+        <v>11.25</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I53" s="2">
+        <v>11.25</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I54" s="2">
+        <v>11.25</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I55" s="2">
+        <v>7.23</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I56" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="2">
+        <v>2</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I57" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I58" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="I59" s="2">
+        <v>2.39</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F60" s="2">
+        <v>1</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" s="2">
+        <v>2</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I62" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="247" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D247" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G247" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="249" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D249" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G249" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="253" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D253" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G253" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="255" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D255" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G255" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:J433">
+  <sortState ref="B2:J481">
     <sortCondition ref="E2:E500"/>
     <sortCondition ref="B2:B500"/>
   </sortState>

</xml_diff>

<commit_message>
addded filter section for discharge measurements.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="407">
   <si>
     <t>PGB1010603MR</t>
   </si>
@@ -88,7 +88,7 @@
     <t>1nF</t>
   </si>
   <si>
-    <t>C23</t>
+    <t>C34</t>
   </si>
   <si>
     <t>CAP CER 1000PF 50V 5% NP0 0805</t>
@@ -103,7 +103,7 @@
     <t>2.2nF</t>
   </si>
   <si>
-    <t>C24</t>
+    <t>C35</t>
   </si>
   <si>
     <t>CAP CER 2200PF 50V 5% NP0 0805</t>
@@ -118,7 +118,7 @@
     <t>15nF</t>
   </si>
   <si>
-    <t>C25</t>
+    <t>C36</t>
   </si>
   <si>
     <t>CAP CER 0.015UF 50V 5% C0G 0805</t>
@@ -139,6 +139,51 @@
     <t>1276-2698-1-ND</t>
   </si>
   <si>
+    <t>CL21C101JBANNNC</t>
+  </si>
+  <si>
+    <t>100pF</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>CAP CER 100PF 50V 5% NP0 0805</t>
+  </si>
+  <si>
+    <t>1276-1014-1-ND</t>
+  </si>
+  <si>
+    <t>CL21C201JBANNNC</t>
+  </si>
+  <si>
+    <t>200pF</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>CAP CER 200PF 50V 5% NP0 0805</t>
+  </si>
+  <si>
+    <t>1276-2601-1-ND</t>
+  </si>
+  <si>
+    <t>CL21C152JBFNNNE</t>
+  </si>
+  <si>
+    <t>1.5nF</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>CAP CER 1500PF 50V 5% NP0 0805</t>
+  </si>
+  <si>
+    <t>1276-2988-1-ND</t>
+  </si>
+  <si>
     <t>GRM1885C1H180FA01D</t>
   </si>
   <si>
@@ -286,19 +331,22 @@
     <t>A34073-ND</t>
   </si>
   <si>
-    <t>HE3621A0510</t>
-  </si>
-  <si>
-    <t>HE3621_NO_SPST</t>
+    <t>SIL05-1A85-76D4K</t>
+  </si>
+  <si>
+    <t>Standex-Meder</t>
+  </si>
+  <si>
+    <t>SPST</t>
   </si>
   <si>
     <t>Relay</t>
   </si>
   <si>
-    <t>RELAY REED SPST 500MA 5V</t>
-  </si>
-  <si>
-    <t>HE207-ND</t>
+    <t>RELAY REED SPST 1A 5V</t>
+  </si>
+  <si>
+    <t>374-1247-ND</t>
   </si>
   <si>
     <t>SDS850R-104M</t>
@@ -316,19 +364,31 @@
     <t>FIXED IND 100UH 500MA 600 MOHM</t>
   </si>
   <si>
+    <t>RNX1251K10FKEL</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>1.1k</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>RES 1.10K OHM 1% 100 PPM 3W</t>
+  </si>
+  <si>
+    <t>RNX1.10KP-ND</t>
+  </si>
+  <si>
     <t>RNX12510M0FKEL</t>
   </si>
   <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
     <t>10M</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R1</t>
+    <t>R2</t>
   </si>
   <si>
     <t>RES 10.0M OHM 1% 100 PPM 3W</t>
@@ -343,7 +403,7 @@
     <t>130k</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>R3</t>
   </si>
   <si>
     <t>RES 130K OHM 1% 100 PPM 5W</t>
@@ -352,18 +412,6 @@
     <t>RNX130KS-ND</t>
   </si>
   <si>
-    <t>RNX1251K10FKEL</t>
-  </si>
-  <si>
-    <t>1.1k</t>
-  </si>
-  <si>
-    <t>RES 1.10K OHM 1% 100 PPM 3W</t>
-  </si>
-  <si>
-    <t>RNX1.10KP-ND</t>
-  </si>
-  <si>
     <t>CRCW12064M99FKEA</t>
   </si>
   <si>
@@ -430,88 +478,178 @@
     <t>4.64k</t>
   </si>
   <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>RES SMD 4.64K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P4.64KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF6491V</t>
+  </si>
+  <si>
+    <t>6.49k</t>
+  </si>
+  <si>
     <t>R17</t>
   </si>
   <si>
-    <t>RES SMD 4.64K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>P4.64KCCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF6491V</t>
-  </si>
-  <si>
-    <t>6.49k</t>
+    <t>RES SMD 6.49K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P6.49KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF2871V</t>
+  </si>
+  <si>
+    <t>2.87k</t>
   </si>
   <si>
     <t>R18</t>
   </si>
   <si>
-    <t>RES SMD 6.49K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>P6.49KCCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF2871V</t>
-  </si>
-  <si>
-    <t>2.87k</t>
+    <t>RES SMD 2.87K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P2.87KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF5361V</t>
+  </si>
+  <si>
+    <t>5.36k</t>
   </si>
   <si>
     <t>R19</t>
   </si>
   <si>
-    <t>RES SMD 2.87K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>P2.87KCCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF5361V</t>
-  </si>
-  <si>
-    <t>5.36k</t>
+    <t>RES SMD 5.36K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P5.36KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1401V</t>
+  </si>
+  <si>
+    <t>1.4k</t>
   </si>
   <si>
     <t>R20</t>
   </si>
   <si>
-    <t>RES SMD 5.36K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>P5.36KCCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF1401V</t>
-  </si>
-  <si>
-    <t>1.4k</t>
+    <t>RES SMD 1.4K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P1.40KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1621V</t>
+  </si>
+  <si>
+    <t>1.62k</t>
   </si>
   <si>
     <t>R21</t>
   </si>
   <si>
-    <t>RES SMD 1.4K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>P1.40KCCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF1621V</t>
-  </si>
-  <si>
-    <t>1.62k</t>
+    <t>RES SMD 1.62K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P1.62KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1182V</t>
+  </si>
+  <si>
+    <t>11.8k</t>
   </si>
   <si>
     <t>R22</t>
   </si>
   <si>
-    <t>RES SMD 1.62K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>P1.62KCCT-ND</t>
+    <t>RES SMD 11.8K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P11.8KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1622V</t>
+  </si>
+  <si>
+    <t>16.2k</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>RES SMD 16.2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P16.2KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF7151V</t>
+  </si>
+  <si>
+    <t>7.15k</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>RES SMD 7.15K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P7.15KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1332V</t>
+  </si>
+  <si>
+    <t>13.3k</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>RES SMD 13.3K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P13.3KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF3481V</t>
+  </si>
+  <si>
+    <t>3.48k</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>RES SMD 3.48K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P3.48KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF4021V</t>
+  </si>
+  <si>
+    <t>4.02k</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>RES SMD 4.02K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>P4.02KCCT-ND</t>
   </si>
   <si>
     <t>ERJ-3EKF1002V</t>
@@ -532,7 +670,7 @@
     <t>50k</t>
   </si>
   <si>
-    <t>R34</t>
+    <t>R39</t>
   </si>
   <si>
     <t>RES SMD 50K OHM 0.02% 1/4W 0805</t>
@@ -547,7 +685,7 @@
     <t>499R</t>
   </si>
   <si>
-    <t>R35</t>
+    <t>R40</t>
   </si>
   <si>
     <t>RES SMD 499 OHM 0.02% 1/4W 0805</t>
@@ -562,7 +700,7 @@
     <t>20k</t>
   </si>
   <si>
-    <t>R36</t>
+    <t>R41</t>
   </si>
   <si>
     <t>RES SMD 20K OHM 0.02% 1/4W 0805</t>
@@ -586,18 +724,18 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>R43</t>
-  </si>
-  <si>
     <t>R44</t>
   </si>
   <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
     <t>ERJ-3EKF5490V</t>
   </si>
   <si>
@@ -616,7 +754,7 @@
     <t>39K</t>
   </si>
   <si>
-    <t>R54</t>
+    <t>R59</t>
   </si>
   <si>
     <t>RES SMD 39K OHM 1% 1/10W 0603</t>
@@ -643,7 +781,7 @@
     <t>2K</t>
   </si>
   <si>
-    <t>R64</t>
+    <t>R69</t>
   </si>
   <si>
     <t>RES SMD 2K OHM 1% 1/10W 0603</t>
@@ -658,7 +796,7 @@
     <t>12k</t>
   </si>
   <si>
-    <t>R65</t>
+    <t>R70</t>
   </si>
   <si>
     <t>RES SMD 12K OHM 1% 1/10W 0603</t>
@@ -733,25 +871,28 @@
     <t>AD817</t>
   </si>
   <si>
+    <t>U3</t>
+  </si>
+  <si>
     <t>IC OPAMP GP 50MHZ 8SOIC</t>
   </si>
   <si>
     <t>AD817ARZ-REEL7CT-ND</t>
   </si>
   <si>
-    <t>LF356MX/NOPB</t>
+    <t>OPA365AMDBVTEP</t>
   </si>
   <si>
     <t>TI</t>
   </si>
   <si>
-    <t>LF356MX</t>
-  </si>
-  <si>
-    <t>IC OPAMP JFET 5MHZ 8SOIC</t>
-  </si>
-  <si>
-    <t>LF356MX/NOPBCT-ND</t>
+    <t>OPA365</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 50MHZ RRO SOT23-5</t>
+  </si>
+  <si>
+    <t>296-29461-1-ND</t>
   </si>
   <si>
     <t>AD7656BSTZ-REEL</t>
@@ -763,7 +904,7 @@
     <t>ADC</t>
   </si>
   <si>
-    <t>U8</t>
+    <t>U10</t>
   </si>
   <si>
     <t>IC ADC 16BIT 6CH 250KSPS 64-LQFP</t>
@@ -796,7 +937,7 @@
     <t>Optocoupler</t>
   </si>
   <si>
-    <t>U11</t>
+    <t>U13</t>
   </si>
   <si>
     <t>OPTOISO 3.75KV PHVOLT 8-FLATPACK</t>
@@ -814,6 +955,9 @@
     <t>Diff Amp</t>
   </si>
   <si>
+    <t>U17</t>
+  </si>
+  <si>
     <t>IC OPAMP DIFF 550KHZ RRO 14SOIC</t>
   </si>
   <si>
@@ -826,12 +970,21 @@
     <t>TLV1702</t>
   </si>
   <si>
+    <t>U18B</t>
+  </si>
+  <si>
     <t>IC COMPARATOR DUAL 8VSSOP</t>
   </si>
   <si>
     <t>296-37236-1-ND</t>
   </si>
   <si>
+    <t>U18A</t>
+  </si>
+  <si>
+    <t>U19</t>
+  </si>
+  <si>
     <t>CD74AC244M96</t>
   </si>
   <si>
@@ -841,6 +994,9 @@
     <t>Buffer</t>
   </si>
   <si>
+    <t>U20</t>
+  </si>
+  <si>
     <t>IC BUFF/DVR TRI-ST DUAL 20SOIC</t>
   </si>
   <si>
@@ -859,7 +1015,7 @@
     <t>Temperature Sensor</t>
   </si>
   <si>
-    <t>U20</t>
+    <t>U21</t>
   </si>
   <si>
     <t>IC SENSOR THERMAL 2.3V SOT-23-3</t>
@@ -880,7 +1036,7 @@
     <t>MCU</t>
   </si>
   <si>
-    <t>U21</t>
+    <t>U22</t>
   </si>
   <si>
     <t>IC MCU ARM M4 32BIT RISC 100LQFP</t>
@@ -901,7 +1057,7 @@
     <t>USB COM</t>
   </si>
   <si>
-    <t>U22</t>
+    <t>U23</t>
   </si>
   <si>
     <t>IC HS USB TO UART/FIFO 48LQFP</t>
@@ -919,7 +1075,7 @@
     <t>RS232 Transceiver</t>
   </si>
   <si>
-    <t>U23</t>
+    <t>U24</t>
   </si>
   <si>
     <t>IC LINE DRVR/RCVR RS232 16-TSSOP</t>
@@ -934,7 +1090,7 @@
     <t>EEPROM</t>
   </si>
   <si>
-    <t>U24</t>
+    <t>U25</t>
   </si>
   <si>
     <t>IC EEPROM 2KBIT 2MHZ SOT23-6</t>
@@ -1009,31 +1165,28 @@
     <t>Qnty</t>
   </si>
   <si>
-    <t>U18, U19</t>
-  </si>
-  <si>
-    <t>C1, C3, C5, C11, C13, C15, C17, C19, C21, C29, C31, C33, C35, C37, C39, C41, C43, C45, C47, C49, C51, C53, C55, C57, C76</t>
-  </si>
-  <si>
-    <t>C2, C4, C6, C10, C12, C14, C16, C18, C20, C22, C30, C32, C34, C36, C38, C40, C42, C44, C46, C48, C50, C52, C54, C56, C58, C59, C60, C61, C62, C63, C64, C65, C66, C67, C68, C69, C70, C71, C72, C73, C74, C75, C81, C82, C83, C84, C85, C86, C87, C90, C91, C92, C93, C95, C96, C98, C102, C104, C106, C108, C109, C110, C111, C112</t>
-  </si>
-  <si>
-    <t>C88, C89, C94, C97</t>
+    <t>C1, C3, C5, C10, C12, C14, C16, C18, C20, C22, C24, C26, C28, C30, C32, C46, C48, C50, C52, C54, C56, C58, C60, C62, C64, C66, C68, C70, C72, C74, C92</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C11, C13, C15, C17, C19, C21, C23, C25, C27, C29, C31, C33, C47, C49, C51, C53, C55, C57, C59, C61, C63, C65, C67, C69, C71, C73, C75, C76, C77, C78, C79, C80, C81, C82, C83, C84, C85, C86, C87, C88, C89, C90, C91, C97, C98, C99, C100, C101, C102, C103, C106, C107, C108, C109, C111, C112, C114, C118, C120, C122, C124, C125, C126, C127, C128</t>
+  </si>
+  <si>
+    <t>C104, C105, C110, C113</t>
   </si>
   <si>
     <t>C7, C8, C9</t>
   </si>
   <si>
-    <t>C26, C27, C28</t>
-  </si>
-  <si>
-    <t>C77, C78, C99, C100</t>
-  </si>
-  <si>
-    <t>C79, C80</t>
-  </si>
-  <si>
-    <t>C101, C103, C105, C107</t>
+    <t>C37, C38, C39, C43, C44, C45</t>
+  </si>
+  <si>
+    <t>C93, C94, C115, C116</t>
+  </si>
+  <si>
+    <t>C95, C96</t>
+  </si>
+  <si>
+    <t>C117, C119, C121, C123</t>
   </si>
   <si>
     <t>J1, J2, J4</t>
@@ -1042,49 +1195,40 @@
     <t>J7, J8</t>
   </si>
   <si>
-    <t>U15, U17</t>
-  </si>
-  <si>
     <t>L1, L2, L3</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
-  </si>
-  <si>
-    <t>U3, U4</t>
-  </si>
-  <si>
-    <t>U5, U6, U7</t>
-  </si>
-  <si>
-    <t>U9, U10, U12, U13, U14</t>
-  </si>
-  <si>
-    <t>U16A, U16B</t>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10</t>
+  </si>
+  <si>
+    <t>U4, U5, U6, U7, U8, U9</t>
+  </si>
+  <si>
+    <t>U11, U12, U14, U15, U16</t>
   </si>
   <si>
     <t>SW1, SW2</t>
   </si>
   <si>
-    <t>LS1, LS2, LS3, LS4, LS5, LS6, LS7, LS8, LS9</t>
-  </si>
-  <si>
-    <t>R8, R9, R10, R11, R12, R13, R14, R15, R16</t>
-  </si>
-  <si>
-    <t>R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R37, R41, R45, R46, R48, R49, R50, R51, R52, R53, R55, R61, R62, R63</t>
-  </si>
-  <si>
-    <t>R56, R58</t>
-  </si>
-  <si>
-    <t>R47, R66</t>
-  </si>
-  <si>
-    <t>R38, R42, R57, R59, R60</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
+    <t>LS1, LS2, LS3, LS4, LS5, LS6, LS7, LS8</t>
+  </si>
+  <si>
+    <t>R8, R9, R10, R11, R12, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R42, R46, R50, R51, R53, R54, R55, R56, R57, R58, R60, R66, R67, R68</t>
+  </si>
+  <si>
+    <t>R61, R63</t>
+  </si>
+  <si>
+    <t>R52, R71</t>
+  </si>
+  <si>
+    <t>R43, R47, R62, R64, R65</t>
+  </si>
+  <si>
+    <t>R1, R4</t>
   </si>
   <si>
     <t>CR1, CR2</t>
@@ -1931,9 +2075,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K255"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1953,37 +2100,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>358</v>
+        <v>406</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>321</v>
+        <v>373</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>322</v>
+        <v>374</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>323</v>
+        <v>375</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>324</v>
+        <v>376</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>330</v>
+        <v>382</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>325</v>
+        <v>377</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>326</v>
+        <v>378</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>327</v>
+        <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>328</v>
+        <v>380</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>329</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1991,25 +2138,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>246</v>
+        <v>293</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>247</v>
+        <v>294</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>248</v>
+        <v>295</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>249</v>
+        <v>296</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
       <c r="I2" s="2">
         <v>24.28</v>
@@ -2018,112 +2165,112 @@
         <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>242</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>273</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>274</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>331</v>
+        <v>383</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>275</v>
+        <v>11</v>
       </c>
       <c r="I3" s="2">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>332</v>
+        <v>384</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2">
-        <v>0.89</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>333</v>
+        <v>385</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="I5" s="2">
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2131,34 +2278,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>334</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="I6" s="2">
-        <v>0.24</v>
+        <v>0.33</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2166,34 +2313,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2201,25 +2348,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>335</v>
+        <v>43</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="I8" s="2">
         <v>0.1</v>
@@ -2228,7 +2375,7 @@
         <v>5</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2271,13 +2418,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>10</v>
@@ -2286,19 +2433,19 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="I10" s="2">
-        <v>0.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2306,34 +2453,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>336</v>
+        <v>48</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I11" s="2">
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2341,34 +2488,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>337</v>
+        <v>29</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="I12" s="2">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2376,25 +2523,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>338</v>
+        <v>387</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2">
         <v>0.1</v>
@@ -2403,7 +2550,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2411,13 +2558,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>10</v>
@@ -2426,159 +2573,159 @@
         <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>339</v>
+        <v>388</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I14" s="2">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <v>731315013</v>
+      <c r="B15" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="I15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="2">
-        <v>3</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="2">
-        <v>2.56</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <v>901512220</v>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>75</v>
+        <v>390</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I16" s="2">
-        <v>5.89</v>
+        <v>0.24</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>68</v>
+      <c r="B17" s="2">
+        <v>731315013</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>71</v>
+        <v>391</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="I17" s="2">
-        <v>0.22</v>
+        <v>2.56</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="2">
+        <v>901512220</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="D18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="I18" s="2">
-        <v>1.39</v>
+        <v>5.89</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2586,34 +2733,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>316</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>310</v>
+        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>317</v>
+        <v>85</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>312</v>
+        <v>80</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>318</v>
+        <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>319</v>
+        <v>87</v>
       </c>
       <c r="I19" s="2">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>320</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2621,34 +2768,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>309</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>310</v>
+        <v>94</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>311</v>
+        <v>95</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>312</v>
+        <v>80</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>313</v>
+        <v>96</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>314</v>
+        <v>97</v>
       </c>
       <c r="I20" s="2">
-        <v>0.44</v>
+        <v>1.39</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>315</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2656,25 +2803,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
       <c r="I21" s="2">
         <v>7.13</v>
@@ -2683,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2691,25 +2838,25 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="F22" s="2">
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>341</v>
+        <v>392</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="I22" s="2">
         <v>3.9</v>
@@ -2718,7 +2865,7 @@
         <v>5</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2726,25 +2873,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>263</v>
+        <v>310</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>265</v>
+        <v>312</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>342</v>
+        <v>313</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>266</v>
+        <v>314</v>
       </c>
       <c r="I23" s="2">
         <v>4.4000000000000004</v>
@@ -2753,7 +2900,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>267</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2761,34 +2908,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>304</v>
+        <v>111</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>278</v>
+        <v>112</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>304</v>
+        <v>113</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>305</v>
+        <v>114</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>306</v>
+        <v>393</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>307</v>
+        <v>115</v>
       </c>
       <c r="I24" s="2">
-        <v>0.27</v>
+        <v>2.48</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>308</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2796,34 +2943,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="F25" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>343</v>
+        <v>394</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="I25" s="2">
-        <v>2.48</v>
+        <v>0.43</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2831,34 +2978,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>283</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>270</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>60</v>
+        <v>284</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>60</v>
+        <v>279</v>
       </c>
       <c r="F26" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>344</v>
+        <v>285</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>61</v>
+        <v>286</v>
       </c>
       <c r="I26" s="2">
-        <v>0.43</v>
+        <v>4.92</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>62</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2866,34 +3013,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F27" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>288</v>
+        <v>395</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="I27" s="2">
-        <v>7.35</v>
+        <v>6.97</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2901,34 +3048,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>237</v>
+        <v>299</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>224</v>
+        <v>277</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>238</v>
+        <v>300</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>233</v>
+        <v>279</v>
       </c>
       <c r="F28" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>345</v>
+        <v>396</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>239</v>
+        <v>301</v>
       </c>
       <c r="I28" s="2">
-        <v>4.92</v>
+        <v>13.2</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>240</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2936,34 +3083,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>243</v>
+        <v>278</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>233</v>
+        <v>279</v>
       </c>
       <c r="F29" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>346</v>
+        <v>280</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="I29" s="2">
-        <v>1.01</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2971,34 +3118,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>231</v>
+        <v>304</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>253</v>
+        <v>305</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>233</v>
+        <v>306</v>
       </c>
       <c r="F30" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>347</v>
+        <v>307</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>254</v>
+        <v>308</v>
       </c>
       <c r="I30" s="2">
-        <v>13.2</v>
+        <v>3.34</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>255</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3006,34 +3153,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>231</v>
+        <v>264</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="F31" s="2">
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>348</v>
+        <v>397</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="I31" s="2">
-        <v>1.75</v>
+        <v>1.51</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3041,34 +3188,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>230</v>
+        <v>105</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>231</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>232</v>
+        <v>107</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>233</v>
+        <v>108</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>234</v>
+        <v>398</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>235</v>
+        <v>109</v>
       </c>
       <c r="I32" s="2">
-        <v>1.1599999999999999</v>
+        <v>9.09</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>236</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3076,34 +3223,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>257</v>
+        <v>133</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>259</v>
+        <v>119</v>
       </c>
       <c r="F33" s="2">
         <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>260</v>
+        <v>135</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>261</v>
+        <v>136</v>
       </c>
       <c r="I33" s="2">
-        <v>3.34</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>262</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3111,69 +3258,69 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>218</v>
+        <v>148</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>219</v>
+        <v>149</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>220</v>
+        <v>119</v>
       </c>
       <c r="F34" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>349</v>
+        <v>399</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="I34" s="2">
-        <v>1.51</v>
+        <v>0.1</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>90</v>
+        <v>212</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>91</v>
+        <v>213</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="F35" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="I35" s="2">
-        <v>2.16</v>
+        <v>0.1</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>94</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3181,34 +3328,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>116</v>
+        <v>258</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>119</v>
+        <v>260</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>120</v>
+        <v>261</v>
       </c>
       <c r="I36" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>121</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3216,25 +3363,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>253</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>133</v>
+        <v>254</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F37" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>351</v>
+        <v>255</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>134</v>
+        <v>256</v>
       </c>
       <c r="I37" s="2">
         <v>0.1</v>
@@ -3243,33 +3390,33 @@
         <v>5</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>166</v>
+        <v>249</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>167</v>
+        <v>250</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F38" s="2">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>352</v>
+        <v>401</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>168</v>
+        <v>251</v>
       </c>
       <c r="I38" s="2">
         <v>0.1</v>
@@ -3278,7 +3425,7 @@
         <v>5</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>169</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3286,25 +3433,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="I39" s="2">
         <v>0.1</v>
@@ -3313,7 +3460,7 @@
         <v>5</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3321,25 +3468,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F40" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>209</v>
+        <v>402</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="I40" s="2">
         <v>0.1</v>
@@ -3348,7 +3495,7 @@
         <v>5</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3356,25 +3503,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F41" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>353</v>
+        <v>403</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>205</v>
+        <v>233</v>
       </c>
       <c r="I41" s="2">
         <v>0.1</v>
@@ -3383,7 +3530,7 @@
         <v>5</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3391,25 +3538,25 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="I42" s="2">
         <v>0.1</v>
@@ -3418,7 +3565,7 @@
         <v>5</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3426,25 +3573,25 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>354</v>
+        <v>199</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I43" s="2">
         <v>0.1</v>
@@ -3453,7 +3600,7 @@
         <v>5</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3461,25 +3608,25 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F44" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>355</v>
+        <v>174</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="I44" s="2">
         <v>0.1</v>
@@ -3488,7 +3635,7 @@
         <v>5</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3496,25 +3643,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="I45" s="2">
         <v>0.1</v>
@@ -3523,7 +3670,7 @@
         <v>5</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3531,25 +3678,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F46" s="2">
         <v>1</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="I46" s="2">
         <v>0.1</v>
@@ -3558,7 +3705,7 @@
         <v>5</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3566,25 +3713,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="I47" s="2">
         <v>0.1</v>
@@ -3593,7 +3740,7 @@
         <v>5</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3601,25 +3748,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>136</v>
+        <v>202</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F48" s="2">
         <v>1</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="I48" s="2">
         <v>0.1</v>
@@ -3628,7 +3775,7 @@
         <v>5</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3636,25 +3783,25 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>151</v>
+        <v>207</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>154</v>
+        <v>210</v>
       </c>
       <c r="I49" s="2">
         <v>0.1</v>
@@ -3663,7 +3810,7 @@
         <v>5</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>155</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3671,25 +3818,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F50" s="2">
         <v>1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="I50" s="2">
         <v>0.1</v>
@@ -3698,7 +3845,7 @@
         <v>5</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3706,34 +3853,34 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="I51" s="2">
-        <v>0.63</v>
+        <v>0.1</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3741,34 +3888,34 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="I52" s="2">
-        <v>11.25</v>
+        <v>0.1</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3776,34 +3923,34 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F53" s="2">
         <v>1</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="I53" s="2">
-        <v>11.25</v>
+        <v>0.1</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3811,34 +3958,34 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="I54" s="2">
-        <v>11.25</v>
+        <v>0.63</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3846,34 +3993,34 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>127</v>
+        <v>226</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D55" s="2">
-        <v>4.7</v>
+        <v>133</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F55" s="2">
         <v>1</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>128</v>
+        <v>228</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>129</v>
+        <v>229</v>
       </c>
       <c r="I55" s="2">
-        <v>7.23</v>
+        <v>11.25</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3881,34 +4028,34 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>100</v>
+        <v>221</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>105</v>
+        <v>224</v>
       </c>
       <c r="I56" s="2">
-        <v>6.4</v>
+        <v>11.25</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3916,34 +4063,34 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>113</v>
+        <v>217</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F57" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>356</v>
+        <v>218</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>114</v>
+        <v>219</v>
       </c>
       <c r="I57" s="2">
-        <v>6.4</v>
+        <v>11.25</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>115</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3951,34 +4098,34 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>108</v>
+        <v>133</v>
+      </c>
+      <c r="D58" s="2">
+        <v>4.7</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F58" s="2">
         <v>1</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="I58" s="2">
-        <v>6.4</v>
+        <v>7.23</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3986,34 +4133,34 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>298</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>242</v>
+        <v>117</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>299</v>
+        <v>123</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>300</v>
+        <v>119</v>
       </c>
       <c r="F59" s="2">
         <v>1</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>301</v>
+        <v>124</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>302</v>
+        <v>125</v>
       </c>
       <c r="I59" s="2">
-        <v>2.39</v>
+        <v>6.4</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>303</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4021,34 +4168,34 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>277</v>
+        <v>116</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>278</v>
+        <v>117</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>279</v>
+        <v>118</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>280</v>
+        <v>119</v>
       </c>
       <c r="F60" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>281</v>
+        <v>404</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>282</v>
+        <v>120</v>
       </c>
       <c r="I60" s="2">
-        <v>0.37</v>
+        <v>6.4</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>283</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4056,34 +4203,34 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F61" s="2">
         <v>1</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F61" s="2">
-        <v>2</v>
-      </c>
       <c r="G61" s="4" t="s">
-        <v>357</v>
+        <v>129</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="I61" s="2">
-        <v>0.67</v>
+        <v>6.4</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -4091,70 +4238,389 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>292</v>
+        <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>293</v>
+        <v>2</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>294</v>
+        <v>3</v>
       </c>
       <c r="F62" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>295</v>
+        <v>405</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>296</v>
+        <v>4</v>
       </c>
       <c r="I62" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="266" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D266" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G266" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="268" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D268" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G268" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="272" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D272" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G272" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="274" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D274" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G274" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="317" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B317" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D317" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E317" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G317" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="H317" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I317" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="J317" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K317" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="319" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B319" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E319" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G319" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="H319" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I319" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="J319" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K319" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="321" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B321" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D321" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E321" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G321" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H321" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I321" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J321" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K321" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="323" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B323" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D323" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E323" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G323" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="H323" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="I323" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="J323" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K323" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="325" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B325" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G325" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="H325" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I325" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="J325" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K325" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="327" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B327" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D327" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E327" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G327" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="H327" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I327" s="2">
+        <v>7.35</v>
+      </c>
+      <c r="J327" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K327" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="329" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B329" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D329" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E329" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="G329" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="H329" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="I329" s="2">
         <v>4.25</v>
       </c>
-      <c r="J62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="247" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D247" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G247" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="249" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D249" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G249" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="253" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D253" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G253" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="255" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D255" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G255" s="4" t="s">
-        <v>193</v>
+      <c r="J329" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K329" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="331" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B331" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E331" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G331" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="H331" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I331" s="2">
+        <v>2.39</v>
+      </c>
+      <c r="J331" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K331" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="333" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B333" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D333" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E333" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G333" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="H333" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="I333" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="J333" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K333" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="335" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B335" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E335" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G335" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="H335" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="I335" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="J335" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K335" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="337" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B337" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D337" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E337" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G337" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="H337" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="I337" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="J337" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K337" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:J481">
+  <sortState ref="B2:J500">
     <sortCondition ref="E2:E500"/>
     <sortCondition ref="B2:B500"/>
   </sortState>

</xml_diff>

<commit_message>
updated board and bom to current design.
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -1165,13 +1165,13 @@
     <t>Qnty</t>
   </si>
   <si>
-    <t>C1, C3, C5, C10, C12, C14, C16, C18, C20, C22, C24, C26, C28, C30, C32, C46, C48, C50, C52, C54, C56, C58, C60, C62, C64, C66, C68, C70, C72, C74, C92</t>
-  </si>
-  <si>
-    <t>C2, C4, C6, C11, C13, C15, C17, C19, C21, C23, C25, C27, C29, C31, C33, C47, C49, C51, C53, C55, C57, C59, C61, C63, C65, C67, C69, C71, C73, C75, C76, C77, C78, C79, C80, C81, C82, C83, C84, C85, C86, C87, C88, C89, C90, C91, C97, C98, C99, C100, C101, C102, C103, C106, C107, C108, C109, C111, C112, C114, C118, C120, C122, C124, C125, C126, C127, C128</t>
-  </si>
-  <si>
-    <t>C104, C105, C110, C113</t>
+    <t>C1, C3, C5, C10, C12, C14, C16, C18, C20, C22, C24, C26, C28, C30, C32, C46, C48, C50, C52, C54, C56, C58, C60, C62, C64, C66, C68, C70, C72, C74, C91</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C11, C13, C15, C17, C19, C21, C23, C25, C27, C29, C31, C33, C47, C49, C51, C53, C55, C57, C59, C61, C63, C65, C67, C69, C71, C73, C75, C76, C77, C78, C79, C80, C81, C82, C83, C84, C85, C86, C87, C88, C89, C90, C96, C97, C98, C99, C100, C101, C102, C105, C106, C107, C108, C110, C111, C113, C117, C119, C121, C123, C124, C125, C126, C127</t>
+  </si>
+  <si>
+    <t>C103, C104, C109, C112</t>
   </si>
   <si>
     <t>C7, C8, C9</t>
@@ -1180,13 +1180,13 @@
     <t>C37, C38, C39, C43, C44, C45</t>
   </si>
   <si>
-    <t>C93, C94, C115, C116</t>
-  </si>
-  <si>
-    <t>C95, C96</t>
-  </si>
-  <si>
-    <t>C117, C119, C121, C123</t>
+    <t>C92, C93, C114, C115</t>
+  </si>
+  <si>
+    <t>C94, C95</t>
+  </si>
+  <si>
+    <t>C116, C118, C120, C122</t>
   </si>
   <si>
     <t>J1, J2, J4</t>
@@ -1216,13 +1216,13 @@
     <t>R8, R9, R10, R11, R12, R13, R14, R15</t>
   </si>
   <si>
-    <t>R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R42, R46, R50, R51, R53, R54, R55, R56, R57, R58, R60, R66, R67, R68</t>
+    <t>R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R42, R46, R50, R52, R53, R54, R55, R56, R57, R58, R60, R66, R67, R68</t>
   </si>
   <si>
     <t>R61, R63</t>
   </si>
   <si>
-    <t>R52, R71</t>
+    <t>R51, R71</t>
   </si>
   <si>
     <t>R43, R47, R62, R64, R65</t>
@@ -2075,12 +2075,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K337"/>
+  <dimension ref="A1:K336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2220,7 +2217,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>384</v>
@@ -3083,13 +3080,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>276</v>
+        <v>316</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>277</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>279</v>
@@ -3098,19 +3095,19 @@
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
       <c r="I29" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.75</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3118,34 +3115,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="I30" s="2">
-        <v>3.34</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3153,34 +3150,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>263</v>
+        <v>303</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>264</v>
+        <v>304</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>265</v>
+        <v>305</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="F31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>397</v>
+        <v>307</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="I31" s="2">
-        <v>1.51</v>
+        <v>3.34</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>268</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3188,34 +3185,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>263</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>106</v>
+        <v>264</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>107</v>
+        <v>265</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>108</v>
+        <v>266</v>
       </c>
       <c r="F32" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>109</v>
+        <v>267</v>
       </c>
       <c r="I32" s="2">
-        <v>9.09</v>
+        <v>1.51</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>110</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3223,34 +3220,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F33" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>135</v>
+        <v>398</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="I33" s="2">
-        <v>1.1000000000000001</v>
+        <v>9.09</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3258,60 +3255,60 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F34" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>399</v>
+        <v>135</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="I34" s="2">
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>212</v>
+        <v>147</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>213</v>
+        <v>149</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F35" s="2">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="I35" s="2">
         <v>0.1</v>
@@ -3320,33 +3317,33 @@
         <v>5</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>258</v>
+        <v>212</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>259</v>
+        <v>213</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F36" s="2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>261</v>
+        <v>214</v>
       </c>
       <c r="I36" s="2">
         <v>0.1</v>
@@ -3355,7 +3352,7 @@
         <v>5</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>262</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3363,13 +3360,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>119</v>
@@ -3378,10 +3375,10 @@
         <v>1</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="I37" s="2">
         <v>0.1</v>
@@ -3390,7 +3387,7 @@
         <v>5</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3398,25 +3395,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F38" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>401</v>
+        <v>255</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="I38" s="2">
         <v>0.1</v>
@@ -3425,7 +3422,7 @@
         <v>5</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3433,25 +3430,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F39" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>246</v>
+        <v>401</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I39" s="2">
         <v>0.1</v>
@@ -3460,7 +3457,7 @@
         <v>5</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3468,25 +3465,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F40" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>402</v>
+        <v>246</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="I40" s="2">
         <v>0.1</v>
@@ -3495,7 +3492,7 @@
         <v>5</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3503,25 +3500,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F41" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="I41" s="2">
         <v>0.1</v>
@@ -3530,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3538,25 +3535,25 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>182</v>
+        <v>231</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F42" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>184</v>
+        <v>403</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="I42" s="2">
         <v>0.1</v>
@@ -3565,7 +3562,7 @@
         <v>5</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3573,13 +3570,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>119</v>
@@ -3588,10 +3585,10 @@
         <v>1</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="I43" s="2">
         <v>0.1</v>
@@ -3600,7 +3597,7 @@
         <v>5</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3608,13 +3605,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>119</v>
@@ -3623,10 +3620,10 @@
         <v>1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="I44" s="2">
         <v>0.1</v>
@@ -3635,7 +3632,7 @@
         <v>5</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3643,13 +3640,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>119</v>
@@ -3658,10 +3655,10 @@
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I45" s="2">
         <v>0.1</v>
@@ -3670,7 +3667,7 @@
         <v>5</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3678,13 +3675,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>119</v>
@@ -3693,10 +3690,10 @@
         <v>1</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I46" s="2">
         <v>0.1</v>
@@ -3705,7 +3702,7 @@
         <v>5</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3713,13 +3710,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>119</v>
@@ -3728,10 +3725,10 @@
         <v>1</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="I47" s="2">
         <v>0.1</v>
@@ -3740,7 +3737,7 @@
         <v>5</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3748,13 +3745,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>119</v>
@@ -3763,10 +3760,10 @@
         <v>1</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="I48" s="2">
         <v>0.1</v>
@@ -3775,7 +3772,7 @@
         <v>5</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3783,13 +3780,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>119</v>
@@ -3798,10 +3795,10 @@
         <v>1</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I49" s="2">
         <v>0.1</v>
@@ -3810,7 +3807,7 @@
         <v>5</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3818,13 +3815,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>153</v>
+        <v>208</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>119</v>
@@ -3833,10 +3830,10 @@
         <v>1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>154</v>
+        <v>209</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>155</v>
+        <v>210</v>
       </c>
       <c r="I50" s="2">
         <v>0.1</v>
@@ -3845,7 +3842,7 @@
         <v>5</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3853,13 +3850,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>119</v>
@@ -3868,10 +3865,10 @@
         <v>1</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="I51" s="2">
         <v>0.1</v>
@@ -3880,7 +3877,7 @@
         <v>5</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3888,13 +3885,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>119</v>
@@ -3903,10 +3900,10 @@
         <v>1</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="I52" s="2">
         <v>0.1</v>
@@ -3915,7 +3912,7 @@
         <v>5</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3923,13 +3920,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>119</v>
@@ -3938,10 +3935,10 @@
         <v>1</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="I53" s="2">
         <v>0.1</v>
@@ -3950,7 +3947,7 @@
         <v>5</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3958,13 +3955,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>192</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>139</v>
+        <v>193</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>119</v>
@@ -3973,19 +3970,19 @@
         <v>1</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>141</v>
+        <v>195</v>
       </c>
       <c r="I54" s="2">
-        <v>0.63</v>
+        <v>0.1</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3993,13 +3990,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>227</v>
+        <v>139</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>119</v>
@@ -4008,19 +4005,19 @@
         <v>1</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>228</v>
+        <v>140</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>229</v>
+        <v>141</v>
       </c>
       <c r="I55" s="2">
-        <v>11.25</v>
+        <v>0.63</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>230</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -4028,13 +4025,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>119</v>
@@ -4043,10 +4040,10 @@
         <v>1</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="I56" s="2">
         <v>11.25</v>
@@ -4055,7 +4052,7 @@
         <v>5</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4063,13 +4060,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>119</v>
@@ -4078,10 +4075,10 @@
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="I57" s="2">
         <v>11.25</v>
@@ -4090,7 +4087,7 @@
         <v>5</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4098,13 +4095,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>143</v>
+        <v>216</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D58" s="2">
-        <v>4.7</v>
+      <c r="D58" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>119</v>
@@ -4113,19 +4110,19 @@
         <v>1</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>144</v>
+        <v>218</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>145</v>
+        <v>219</v>
       </c>
       <c r="I58" s="2">
-        <v>7.23</v>
+        <v>11.25</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>146</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4133,13 +4130,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>123</v>
+        <v>133</v>
+      </c>
+      <c r="D59" s="2">
+        <v>4.7</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>119</v>
@@ -4148,19 +4145,19 @@
         <v>1</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="I59" s="2">
-        <v>6.4</v>
+        <v>7.23</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4168,25 +4165,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F60" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>404</v>
+        <v>124</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="I60" s="2">
         <v>6.4</v>
@@ -4195,7 +4192,7 @@
         <v>5</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4203,25 +4200,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F61" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>129</v>
+        <v>404</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I61" s="2">
         <v>6.4</v>
@@ -4230,7 +4227,7 @@
         <v>5</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -4238,33 +4235,68 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I62" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F63" s="2">
         <v>2</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G63" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I63" s="2">
         <v>0.67</v>
       </c>
-      <c r="J62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K62" s="2" t="s">
+      <c r="J63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K63" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4300,322 +4332,293 @@
         <v>239</v>
       </c>
     </row>
-    <row r="317" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B317" s="2" t="s">
+    <row r="318" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B318" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C317" s="2" t="s">
+      <c r="C318" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D317" s="2" t="s">
+      <c r="D318" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="E317" s="2" t="s">
+      <c r="E318" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G317" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="H317" s="2" t="s">
+      <c r="G318" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="H318" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="I317" s="2">
+      <c r="I318" s="2">
         <v>1.75</v>
       </c>
-      <c r="J317" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K317" s="2" t="s">
+      <c r="J318" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K318" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="319" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B319" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C319" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D319" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E319" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="G319" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="H319" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="I319" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="J319" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K319" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="321" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B321" s="2" t="s">
+    <row r="320" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B320" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C321" s="2" t="s">
+      <c r="C320" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="D321" s="2" t="s">
+      <c r="D320" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E321" s="2" t="s">
+      <c r="E320" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G321" s="4" t="s">
+      <c r="G320" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="H321" s="2" t="s">
+      <c r="H320" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="I321" s="2">
+      <c r="I320" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J321" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K321" s="2" t="s">
+      <c r="J320" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K320" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="323" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B323" s="2" t="s">
+    <row r="322" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B322" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C323" s="2" t="s">
+      <c r="C322" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D323" s="2" t="s">
+      <c r="D322" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="E323" s="2" t="s">
+      <c r="E322" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G323" s="4" t="s">
+      <c r="G322" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="H323" s="2" t="s">
+      <c r="H322" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I323" s="2">
+      <c r="I322" s="2">
         <v>0.91</v>
       </c>
-      <c r="J323" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K323" s="2" t="s">
+      <c r="J322" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K322" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="325" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B325" s="2" t="s">
+    <row r="324" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B324" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C325" s="2" t="s">
+      <c r="C324" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D325" s="2" t="s">
+      <c r="D324" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E325" s="2" t="s">
+      <c r="E324" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="G325" s="4" t="s">
+      <c r="G324" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="H325" s="2" t="s">
+      <c r="H324" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="I325" s="2">
+      <c r="I324" s="2">
         <v>0.37</v>
       </c>
-      <c r="J325" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K325" s="2" t="s">
+      <c r="J324" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K324" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="327" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B327" s="2" t="s">
+    <row r="326" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B326" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C327" s="2" t="s">
+      <c r="C326" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D327" s="2" t="s">
+      <c r="D326" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="E327" s="2" t="s">
+      <c r="E326" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="G327" s="4" t="s">
+      <c r="G326" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H327" s="2" t="s">
+      <c r="H326" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="I327" s="2">
+      <c r="I326" s="2">
         <v>7.35</v>
       </c>
-      <c r="J327" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K327" s="2" t="s">
+      <c r="J326" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K326" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="329" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B329" s="2" t="s">
+    <row r="328" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B328" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C329" s="2" t="s">
+      <c r="C328" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D329" s="2" t="s">
+      <c r="D328" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E329" s="2" t="s">
+      <c r="E328" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="G329" s="4" t="s">
+      <c r="G328" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="H329" s="2" t="s">
+      <c r="H328" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="I329" s="2">
+      <c r="I328" s="2">
         <v>4.25</v>
       </c>
-      <c r="J329" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K329" s="2" t="s">
+      <c r="J328" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K328" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="331" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B331" s="2" t="s">
+    <row r="330" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B330" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C331" s="2" t="s">
+      <c r="C330" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D331" s="2" t="s">
+      <c r="D330" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="E331" s="2" t="s">
+      <c r="E330" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G331" s="4" t="s">
+      <c r="G330" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="H331" s="2" t="s">
+      <c r="H330" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="I331" s="2">
+      <c r="I330" s="2">
         <v>2.39</v>
       </c>
-      <c r="J331" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K331" s="2" t="s">
+      <c r="J330" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K330" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="333" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B333" s="2" t="s">
+    <row r="332" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B332" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C333" s="2" t="s">
+      <c r="C332" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D333" s="2" t="s">
+      <c r="D332" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="E333" s="2" t="s">
+      <c r="E332" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="G333" s="4" t="s">
+      <c r="G332" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="H333" s="2" t="s">
+      <c r="H332" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="I333" s="2">
+      <c r="I332" s="2">
         <v>0.27</v>
       </c>
-      <c r="J333" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K333" s="2" t="s">
+      <c r="J332" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K332" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="335" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B335" s="2" t="s">
+    <row r="334" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B334" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C335" s="2" t="s">
+      <c r="C334" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D335" s="2" t="s">
+      <c r="D334" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="E335" s="2" t="s">
+      <c r="E334" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="G335" s="4" t="s">
+      <c r="G334" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="H335" s="2" t="s">
+      <c r="H334" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="I335" s="2">
+      <c r="I334" s="2">
         <v>0.44</v>
       </c>
-      <c r="J335" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K335" s="2" t="s">
+      <c r="J334" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K334" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="337" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B337" s="2" t="s">
+    <row r="336" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B336" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C337" s="2" t="s">
+      <c r="C336" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D337" s="2" t="s">
+      <c r="D336" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="E337" s="2" t="s">
+      <c r="E336" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="G337" s="4" t="s">
+      <c r="G336" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="H337" s="2" t="s">
+      <c r="H336" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="I337" s="2">
+      <c r="I336" s="2">
         <v>0.44</v>
       </c>
-      <c r="J337" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K337" s="2" t="s">
+      <c r="J336" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K336" s="2" t="s">
         <v>372</v>
       </c>
     </row>

</xml_diff>